<commit_message>
modified unnamed 0 always empty for State in child mortality sheet
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D698AD6-3C4F-47BD-B39B-DAB857C554E4}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB6D851-15F1-4697-B6D3-25C008CDB7AE}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="17" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
@@ -11550,17 +11550,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16579,17 +16579,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -21627,11 +21627,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -21640,6 +21635,11 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31609,6 +31609,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -31616,13 +31623,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -36615,6 +36615,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -36622,13 +36629,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36639,7 +36639,7 @@
   <dimension ref="A2:U81"/>
   <sheetViews>
     <sheetView zoomScale="56" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41620,6 +41620,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -41627,13 +41634,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41643,8 +41643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BJ38" sqref="BJ38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41653,6 +41653,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:62" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>118</v>
+      </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
@@ -41725,9 +41728,6 @@
       <c r="BI2" s="45"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
-        <v>118</v>
-      </c>
       <c r="B3" s="45" t="s">
         <v>1</v>
       </c>
@@ -53049,6 +53049,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="G36:P36"/>
+    <mergeCell ref="Q36:Z36"/>
+    <mergeCell ref="AA36:AJ36"/>
+    <mergeCell ref="AO36:AT36"/>
+    <mergeCell ref="AY36:BI36"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="AZ3:BD3"/>
     <mergeCell ref="BE37:BI37"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="G37:K37"/>
@@ -53061,28 +53083,6 @@
     <mergeCell ref="AP37:AT37"/>
     <mergeCell ref="AU37:AY37"/>
     <mergeCell ref="AZ37:BD37"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="G36:P36"/>
-    <mergeCell ref="Q36:Z36"/>
-    <mergeCell ref="AA36:AJ36"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AY36:BI36"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AU3:AY3"/>
-    <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60448,6 +60448,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60456,11 +60461,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -65423,6 +65423,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -65430,13 +65437,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70398,17 +70398,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75411,17 +75411,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -80679,17 +80679,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -85711,17 +85711,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -90686,17 +90686,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -95691,16 +95691,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
missing daman diu in measles
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DB6D851-15F1-4697-B6D3-25C008CDB7AE}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF4EAD0E-9DFD-44E5-94AB-9041A27BB5B2}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="17" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="13" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3585" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="153">
   <si>
     <t>State/UTs</t>
   </si>
@@ -11550,17 +11550,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16579,17 +16579,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -21627,6 +21627,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -21635,11 +21640,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21649,8 +21649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C819A898-07DF-4DD7-ACE7-420CEFEDBECF}">
   <dimension ref="A2:Z83"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V55" sqref="V55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24807,9 +24807,7 @@
       <c r="U55" t="s">
         <v>70</v>
       </c>
-      <c r="V55" s="14" t="s">
-        <v>115</v>
-      </c>
+      <c r="V55" s="14"/>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
@@ -31609,6 +31607,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -31616,13 +31621,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -36615,6 +36613,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -36622,13 +36627,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41620,6 +41618,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -41627,13 +41632,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41643,7 +41641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -53049,16 +53047,18 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE37:BI37"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="L37:P37"/>
+    <mergeCell ref="Q37:U37"/>
+    <mergeCell ref="V37:Z37"/>
+    <mergeCell ref="AA37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AT37"/>
+    <mergeCell ref="AU37:AY37"/>
+    <mergeCell ref="AZ37:BD37"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="G36:P36"/>
     <mergeCell ref="Q36:Z36"/>
@@ -53071,18 +53071,16 @@
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AU3:AY3"/>
     <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="BE37:BI37"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="L37:P37"/>
-    <mergeCell ref="Q37:U37"/>
-    <mergeCell ref="V37:Z37"/>
-    <mergeCell ref="AA37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AT37"/>
-    <mergeCell ref="AU37:AY37"/>
-    <mergeCell ref="AZ37:BD37"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60448,11 +60446,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60461,6 +60454,11 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -65423,6 +65421,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -65430,13 +65435,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70398,17 +70396,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75411,17 +75409,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -80679,17 +80677,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -85711,17 +85709,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -90686,17 +90684,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -95691,16 +95689,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
address possible data columns in equity by category of disaggregation
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF4EAD0E-9DFD-44E5-94AB-9041A27BB5B2}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4321E6F5-E1E7-47CB-BD30-D4F36E5FD848}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="13" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3584" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="154">
   <si>
     <t>State/UTs</t>
   </si>
@@ -514,6 +514,9 @@
   <si>
     <t>Childhood</t>
   </si>
+  <si>
+    <t>Equity_Categories</t>
+  </si>
 </sst>
 </file>
 
@@ -611,7 +614,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -671,11 +674,184 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -818,6 +994,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1132,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,263 +1334,330 @@
     <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="53" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="E1" s="57" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="C2" t="str">
+      <c r="C2" s="64" t="str">
         <f>B2</f>
         <v>Any ANC</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="E2" s="59" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C3" s="54" t="str">
         <f t="shared" ref="C3:C17" si="0">B3</f>
         <v>ANC4+</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="E3" s="59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="56" t="s">
         <v>132</v>
       </c>
-      <c r="C4" t="str">
+      <c r="C4" s="54" t="str">
         <f t="shared" si="0"/>
         <v>IFA for 100 days</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="E4" s="59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="58" t="s">
         <v>147</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="56" t="s">
         <v>133</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="54" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="E5" s="59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C6" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Institutional delivery</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="E6" s="59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="58" t="s">
         <v>149</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="C7" t="str">
+      <c r="C7" s="54" t="str">
         <f t="shared" si="0"/>
         <v>C-section delivery</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="E7" s="59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="56" t="s">
         <v>136</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C8" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Breastfeeding 1 hour</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="E8" s="59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="C9" t="str">
+      <c r="C9" s="54" t="str">
         <f t="shared" si="0"/>
         <v>PNC mother 2 days</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="E9" s="59" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="56" t="s">
         <v>138</v>
       </c>
-      <c r="C10" t="str">
+      <c r="C10" s="54" t="str">
         <f t="shared" si="0"/>
         <v>PNC children 2 days</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="E10" s="59" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="56" t="s">
         <v>139</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="54" t="str">
         <f t="shared" si="0"/>
         <v>DPT3</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="E11" s="59" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="56" t="s">
         <v>140</v>
       </c>
-      <c r="C12" t="str">
+      <c r="C12" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Immunisation</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="E12" s="59" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="56" t="s">
         <v>141</v>
       </c>
-      <c r="C13" t="str">
+      <c r="C13" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Diarrhoea</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="E13" s="59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="56" t="s">
         <v>142</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C14" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Measles</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="E14" s="59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="56" t="s">
         <v>143</v>
       </c>
-      <c r="C15" t="str">
+      <c r="C15" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Stunted</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="E15" s="59" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="C16" t="str">
+      <c r="C16" s="54" t="str">
         <f t="shared" si="0"/>
         <v>Wasted</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="E16" s="59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="56" t="s">
         <v>145</v>
       </c>
-      <c r="C17" t="str">
+      <c r="C17" s="61" t="str">
         <f t="shared" si="0"/>
         <v>Underweight</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="E17" s="59" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="54" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="E18" s="59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="54" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
+      <c r="E19" s="59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="54" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
+      <c r="E20" s="59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="65" t="s">
         <v>125</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="E21" s="59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="55" t="s">
         <v>126</v>
+      </c>
+      <c r="E22" s="60" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -11550,17 +11808,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16579,17 +16837,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -21627,11 +21885,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -21640,6 +21893,11 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21649,8 +21907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C819A898-07DF-4DD7-ACE7-420CEFEDBECF}">
   <dimension ref="A2:Z83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V55" sqref="V55"/>
+    <sheetView topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31607,6 +31865,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -31614,13 +31879,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -36613,6 +36871,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -36620,13 +36885,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41618,6 +41876,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -41625,13 +41890,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53047,6 +53305,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="G36:P36"/>
+    <mergeCell ref="Q36:Z36"/>
+    <mergeCell ref="AA36:AJ36"/>
+    <mergeCell ref="AO36:AT36"/>
+    <mergeCell ref="AY36:BI36"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="AZ3:BD3"/>
     <mergeCell ref="BE37:BI37"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="G37:K37"/>
@@ -53059,28 +53339,6 @@
     <mergeCell ref="AP37:AT37"/>
     <mergeCell ref="AU37:AY37"/>
     <mergeCell ref="AZ37:BD37"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="G36:P36"/>
-    <mergeCell ref="Q36:Z36"/>
-    <mergeCell ref="AA36:AJ36"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AY36:BI36"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AU3:AY3"/>
-    <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60446,6 +60704,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60454,11 +60717,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -65421,6 +65679,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -65428,13 +65693,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -70396,17 +70654,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75409,17 +75667,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -80677,17 +80935,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -85709,17 +85967,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -90684,17 +90942,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -95689,16 +95947,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified year label always first above data - empty space eliminated between data and year label in child mortality sheet
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4321E6F5-E1E7-47CB-BD30-D4F36E5FD848}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5415FB8-6E42-4141-BC80-91252DE6A36B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="17" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -614,7 +614,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -847,6 +847,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -940,6 +951,20 @@
       <alignment horizontal="right" vertical="top" indent="2" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,21 +1019,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,7 +1338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -1338,325 +1351,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="39" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="64" t="str">
+      <c r="C2" s="46" t="str">
         <f>B2</f>
         <v>Any ANC</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="41" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="54" t="str">
+      <c r="C3" s="36" t="str">
         <f t="shared" ref="C3:C17" si="0">B3</f>
         <v>ANC4+</v>
       </c>
-      <c r="E3" s="59" t="s">
+      <c r="E3" s="41" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="54" t="str">
+      <c r="C4" s="36" t="str">
         <f t="shared" si="0"/>
         <v>IFA for 100 days</v>
       </c>
-      <c r="E4" s="59" t="s">
+      <c r="E4" s="41" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="41" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="54" t="str">
+      <c r="C6" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Institutional delivery</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="41" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="58" t="s">
+      <c r="A7" s="40" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="54" t="str">
+      <c r="C7" s="36" t="str">
         <f t="shared" si="0"/>
         <v>C-section delivery</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="41" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="54" t="str">
+      <c r="C8" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Breastfeeding 1 hour</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="41" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="54" t="str">
+      <c r="C9" s="36" t="str">
         <f t="shared" si="0"/>
         <v>PNC mother 2 days</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="41" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="58" t="s">
+      <c r="A10" s="40" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="56" t="s">
+      <c r="B10" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="54" t="str">
+      <c r="C10" s="36" t="str">
         <f t="shared" si="0"/>
         <v>PNC children 2 days</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="54" t="str">
+      <c r="C11" s="36" t="str">
         <f t="shared" si="0"/>
         <v>DPT3</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="41" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="54" t="str">
+      <c r="C12" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Immunisation</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="41" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="54" t="str">
+      <c r="C13" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Diarrhoea</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="E13" s="41" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="40" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="54" t="str">
+      <c r="C14" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Measles</v>
       </c>
-      <c r="E14" s="59" t="s">
+      <c r="E14" s="41" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="38" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="54" t="str">
+      <c r="C15" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Stunted</v>
       </c>
-      <c r="E15" s="59" t="s">
+      <c r="E15" s="41" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="58" t="s">
+      <c r="A16" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="54" t="str">
+      <c r="C16" s="36" t="str">
         <f t="shared" si="0"/>
         <v>Wasted</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="41" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="58" t="s">
+      <c r="A17" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="61" t="str">
+      <c r="C17" s="43" t="str">
         <f t="shared" si="0"/>
         <v>Underweight</v>
       </c>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="41" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="54" t="s">
+      <c r="C18" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="41" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B19" s="65" t="s">
+      <c r="B19" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="54" t="s">
+      <c r="C19" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="59" t="s">
+      <c r="E19" s="41" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B20" s="65" t="s">
+      <c r="B20" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="54" t="s">
+      <c r="C20" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="59" t="s">
+      <c r="E20" s="41" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="59" t="s">
+      <c r="A21" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B21" s="65" t="s">
+      <c r="B21" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="41" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="60" t="s">
+      <c r="A22" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="37" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="42" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1683,65 +1696,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:26" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -4249,34 +4262,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="49"/>
+      <c r="E43" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35" t="s">
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35" t="s">
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="34" t="s">
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
@@ -6780,57 +6793,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -9336,34 +9349,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="49"/>
+      <c r="E43" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35" t="s">
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35" t="s">
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="34" t="s">
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AL43" s="2"/>
@@ -11808,17 +11821,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11840,59 +11853,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -14380,34 +14393,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="49"/>
+      <c r="E43" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35" t="s">
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35" t="s">
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="34" t="s">
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -16837,17 +16850,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -16871,64 +16884,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="42"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -19386,34 +19399,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -21885,6 +21898,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -21893,11 +21911,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21920,44 +21933,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="42"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -24397,44 +24410,44 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="44"/>
-      <c r="E45" s="44" t="s">
+      <c r="D45" s="58"/>
+      <c r="E45" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44" t="s">
+      <c r="F45" s="58"/>
+      <c r="G45" s="58"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="58"/>
+      <c r="J45" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="44"/>
-      <c r="L45" s="44"/>
-      <c r="M45" s="44"/>
-      <c r="N45" s="44" t="s">
+      <c r="K45" s="58"/>
+      <c r="L45" s="58"/>
+      <c r="M45" s="58"/>
+      <c r="N45" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O45" s="44"/>
-      <c r="P45" s="44"/>
-      <c r="Q45" s="44"/>
-      <c r="R45" s="43" t="s">
+      <c r="O45" s="58"/>
+      <c r="P45" s="58"/>
+      <c r="Q45" s="58"/>
+      <c r="R45" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="43"/>
-      <c r="T45" s="43"/>
+      <c r="S45" s="57"/>
+      <c r="T45" s="57"/>
     </row>
     <row r="46" spans="1:26" ht="28" x14ac:dyDescent="0.35">
-      <c r="A46" s="44"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
@@ -26890,44 +26903,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -29371,44 +29384,44 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="58"/>
+      <c r="E42" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="58"/>
+      <c r="J42" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="58"/>
+      <c r="L42" s="58"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="58"/>
+      <c r="P42" s="58"/>
+      <c r="Q42" s="58"/>
+      <c r="R42" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A43" s="44"/>
-      <c r="B43" s="44"/>
+      <c r="A43" s="58"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="11" t="s">
         <v>7</v>
       </c>
@@ -31865,6 +31878,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -31872,13 +31892,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31896,44 +31909,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -34377,44 +34390,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="58"/>
+      <c r="E43" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="44"/>
-      <c r="B44" s="44"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -36871,6 +36884,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -36878,13 +36898,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36901,44 +36914,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="57"/>
+      <c r="T2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -39382,44 +39395,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="44" t="s">
+      <c r="B43" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="58"/>
+      <c r="E43" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="58"/>
+      <c r="G43" s="58"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="58"/>
+      <c r="J43" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="58"/>
+      <c r="L43" s="58"/>
+      <c r="M43" s="58"/>
+      <c r="N43" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="58"/>
+      <c r="P43" s="58"/>
+      <c r="Q43" s="58"/>
+      <c r="R43" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="44"/>
-      <c r="B44" s="44"/>
+      <c r="A44" s="58"/>
+      <c r="B44" s="58"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -41876,6 +41889,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -41883,13 +41903,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41899,8 +41912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AX23" workbookViewId="0">
+      <selection activeCell="BJ38" sqref="BJ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41917,160 +41930,158 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46" t="s">
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="45" t="s">
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="61"/>
+      <c r="V2" s="61"/>
+      <c r="W2" s="61"/>
+      <c r="X2" s="61"/>
+      <c r="Y2" s="61"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="45"/>
-      <c r="AC2" s="45"/>
-      <c r="AD2" s="45"/>
-      <c r="AE2" s="45"/>
-      <c r="AF2" s="45"/>
-      <c r="AG2" s="45"/>
-      <c r="AH2" s="45"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="45"/>
+      <c r="AB2" s="59"/>
+      <c r="AC2" s="59"/>
+      <c r="AD2" s="59"/>
+      <c r="AE2" s="59"/>
+      <c r="AF2" s="59"/>
+      <c r="AG2" s="59"/>
+      <c r="AH2" s="59"/>
+      <c r="AI2" s="59"/>
+      <c r="AJ2" s="59"/>
       <c r="AK2" s="29"/>
       <c r="AL2" s="29"/>
       <c r="AM2" s="29"/>
       <c r="AN2" s="29"/>
-      <c r="AO2" s="49" t="s">
+      <c r="AO2" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" s="50"/>
-      <c r="AQ2" s="50"/>
-      <c r="AR2" s="50"/>
-      <c r="AS2" s="50"/>
-      <c r="AT2" s="51"/>
+      <c r="AP2" s="64"/>
+      <c r="AQ2" s="64"/>
+      <c r="AR2" s="64"/>
+      <c r="AS2" s="64"/>
+      <c r="AT2" s="65"/>
       <c r="AU2" s="23"/>
       <c r="AV2" s="23"/>
       <c r="AW2" s="23"/>
       <c r="AX2" s="23"/>
-      <c r="AY2" s="45" t="s">
+      <c r="AY2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AZ2" s="45"/>
-      <c r="BA2" s="45"/>
-      <c r="BB2" s="45"/>
-      <c r="BC2" s="45"/>
-      <c r="BD2" s="45"/>
-      <c r="BE2" s="45"/>
-      <c r="BF2" s="45"/>
-      <c r="BG2" s="45"/>
-      <c r="BH2" s="45"/>
-      <c r="BI2" s="45"/>
+      <c r="AZ2" s="59"/>
+      <c r="BA2" s="59"/>
+      <c r="BB2" s="59"/>
+      <c r="BC2" s="59"/>
+      <c r="BD2" s="59"/>
+      <c r="BE2" s="59"/>
+      <c r="BF2" s="59"/>
+      <c r="BG2" s="59"/>
+      <c r="BH2" s="59"/>
+      <c r="BI2" s="59"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45" t="s">
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45" t="s">
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45" t="s">
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45" t="s">
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45" t="s">
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="59"/>
+      <c r="Z3" s="59"/>
+      <c r="AA3" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45" t="s">
+      <c r="AB3" s="59"/>
+      <c r="AC3" s="59"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="59"/>
+      <c r="AF3" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45" t="s">
+      <c r="AG3" s="59"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="59"/>
+      <c r="AJ3" s="59"/>
+      <c r="AK3" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="45"/>
-      <c r="AP3" s="45" t="s">
+      <c r="AL3" s="59"/>
+      <c r="AM3" s="59"/>
+      <c r="AN3" s="59"/>
+      <c r="AO3" s="59"/>
+      <c r="AP3" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="45"/>
-      <c r="AR3" s="45"/>
-      <c r="AS3" s="45"/>
-      <c r="AT3" s="45"/>
-      <c r="AU3" s="45" t="s">
+      <c r="AQ3" s="59"/>
+      <c r="AR3" s="59"/>
+      <c r="AS3" s="59"/>
+      <c r="AT3" s="59"/>
+      <c r="AU3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="45"/>
-      <c r="AW3" s="45"/>
-      <c r="AX3" s="45"/>
-      <c r="AY3" s="45"/>
-      <c r="AZ3" s="45" t="s">
+      <c r="AV3" s="59"/>
+      <c r="AW3" s="59"/>
+      <c r="AX3" s="59"/>
+      <c r="AY3" s="59"/>
+      <c r="AZ3" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="BA3" s="45"/>
-      <c r="BB3" s="45"/>
-      <c r="BC3" s="45"/>
-      <c r="BD3" s="45"/>
-      <c r="BE3" s="45" t="s">
+      <c r="BA3" s="59"/>
+      <c r="BB3" s="59"/>
+      <c r="BC3" s="59"/>
+      <c r="BD3" s="59"/>
+      <c r="BE3" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="45"/>
-      <c r="BG3" s="45"/>
-      <c r="BH3" s="45"/>
-      <c r="BI3" s="45"/>
-      <c r="BJ3" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF3" s="59"/>
+      <c r="BG3" s="59"/>
+      <c r="BH3" s="59"/>
+      <c r="BI3" s="59"/>
+      <c r="BJ3" s="1"/>
     </row>
     <row r="4" spans="1:62" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
@@ -42253,6 +42264,9 @@
       </c>
       <c r="BI4" s="24" t="s">
         <v>126</v>
+      </c>
+      <c r="BJ4" s="66" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.35">
@@ -47587,163 +47601,161 @@
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="45" t="s">
+      <c r="G36" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="46" t="s">
+      <c r="H36" s="59"/>
+      <c r="I36" s="59"/>
+      <c r="J36" s="59"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="59"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="47"/>
-      <c r="V36" s="47"/>
-      <c r="W36" s="47"/>
-      <c r="X36" s="47"/>
-      <c r="Y36" s="47"/>
-      <c r="Z36" s="48"/>
-      <c r="AA36" s="45" t="s">
+      <c r="R36" s="61"/>
+      <c r="S36" s="61"/>
+      <c r="T36" s="61"/>
+      <c r="U36" s="61"/>
+      <c r="V36" s="61"/>
+      <c r="W36" s="61"/>
+      <c r="X36" s="61"/>
+      <c r="Y36" s="61"/>
+      <c r="Z36" s="62"/>
+      <c r="AA36" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="AB36" s="45"/>
-      <c r="AC36" s="45"/>
-      <c r="AD36" s="45"/>
-      <c r="AE36" s="45"/>
-      <c r="AF36" s="45"/>
-      <c r="AG36" s="45"/>
-      <c r="AH36" s="45"/>
-      <c r="AI36" s="45"/>
-      <c r="AJ36" s="45"/>
+      <c r="AB36" s="59"/>
+      <c r="AC36" s="59"/>
+      <c r="AD36" s="59"/>
+      <c r="AE36" s="59"/>
+      <c r="AF36" s="59"/>
+      <c r="AG36" s="59"/>
+      <c r="AH36" s="59"/>
+      <c r="AI36" s="59"/>
+      <c r="AJ36" s="59"/>
       <c r="AK36" s="29"/>
       <c r="AL36" s="29"/>
       <c r="AM36" s="29"/>
       <c r="AN36" s="29"/>
-      <c r="AO36" s="49" t="s">
+      <c r="AO36" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="AP36" s="50"/>
-      <c r="AQ36" s="50"/>
-      <c r="AR36" s="50"/>
-      <c r="AS36" s="50"/>
-      <c r="AT36" s="51"/>
+      <c r="AP36" s="64"/>
+      <c r="AQ36" s="64"/>
+      <c r="AR36" s="64"/>
+      <c r="AS36" s="64"/>
+      <c r="AT36" s="65"/>
       <c r="AU36" s="23"/>
       <c r="AV36" s="23"/>
       <c r="AW36" s="23"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="45" t="s">
+      <c r="AY36" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AZ36" s="45"/>
-      <c r="BA36" s="45"/>
-      <c r="BB36" s="45"/>
-      <c r="BC36" s="45"/>
-      <c r="BD36" s="45"/>
-      <c r="BE36" s="45"/>
-      <c r="BF36" s="45"/>
-      <c r="BG36" s="45"/>
-      <c r="BH36" s="45"/>
-      <c r="BI36" s="45"/>
+      <c r="AZ36" s="59"/>
+      <c r="BA36" s="59"/>
+      <c r="BB36" s="59"/>
+      <c r="BC36" s="59"/>
+      <c r="BD36" s="59"/>
+      <c r="BE36" s="59"/>
+      <c r="BF36" s="59"/>
+      <c r="BG36" s="59"/>
+      <c r="BH36" s="59"/>
+      <c r="BI36" s="59"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="45" t="s">
+      <c r="B37" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="45"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45" t="s">
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45" t="s">
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45" t="s">
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="45" t="s">
+      <c r="R37" s="59"/>
+      <c r="S37" s="59"/>
+      <c r="T37" s="59"/>
+      <c r="U37" s="59"/>
+      <c r="V37" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="W37" s="45"/>
-      <c r="X37" s="45"/>
-      <c r="Y37" s="45"/>
-      <c r="Z37" s="45"/>
-      <c r="AA37" s="45" t="s">
+      <c r="W37" s="59"/>
+      <c r="X37" s="59"/>
+      <c r="Y37" s="59"/>
+      <c r="Z37" s="59"/>
+      <c r="AA37" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AB37" s="45"/>
-      <c r="AC37" s="45"/>
-      <c r="AD37" s="45"/>
-      <c r="AE37" s="45"/>
-      <c r="AF37" s="45" t="s">
+      <c r="AB37" s="59"/>
+      <c r="AC37" s="59"/>
+      <c r="AD37" s="59"/>
+      <c r="AE37" s="59"/>
+      <c r="AF37" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="AG37" s="45"/>
-      <c r="AH37" s="45"/>
-      <c r="AI37" s="45"/>
-      <c r="AJ37" s="45"/>
-      <c r="AK37" s="45" t="s">
+      <c r="AG37" s="59"/>
+      <c r="AH37" s="59"/>
+      <c r="AI37" s="59"/>
+      <c r="AJ37" s="59"/>
+      <c r="AK37" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="AL37" s="45"/>
-      <c r="AM37" s="45"/>
-      <c r="AN37" s="45"/>
-      <c r="AO37" s="45"/>
-      <c r="AP37" s="45" t="s">
+      <c r="AL37" s="59"/>
+      <c r="AM37" s="59"/>
+      <c r="AN37" s="59"/>
+      <c r="AO37" s="59"/>
+      <c r="AP37" s="59" t="s">
         <v>23</v>
       </c>
-      <c r="AQ37" s="45"/>
-      <c r="AR37" s="45"/>
-      <c r="AS37" s="45"/>
-      <c r="AT37" s="45"/>
-      <c r="AU37" s="45" t="s">
+      <c r="AQ37" s="59"/>
+      <c r="AR37" s="59"/>
+      <c r="AS37" s="59"/>
+      <c r="AT37" s="59"/>
+      <c r="AU37" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="AV37" s="45"/>
-      <c r="AW37" s="45"/>
-      <c r="AX37" s="45"/>
-      <c r="AY37" s="45"/>
-      <c r="AZ37" s="45" t="s">
+      <c r="AV37" s="59"/>
+      <c r="AW37" s="59"/>
+      <c r="AX37" s="59"/>
+      <c r="AY37" s="59"/>
+      <c r="AZ37" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="BA37" s="45"/>
-      <c r="BB37" s="45"/>
-      <c r="BC37" s="45"/>
-      <c r="BD37" s="45"/>
-      <c r="BE37" s="45" t="s">
+      <c r="BA37" s="59"/>
+      <c r="BB37" s="59"/>
+      <c r="BC37" s="59"/>
+      <c r="BD37" s="59"/>
+      <c r="BE37" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="BF37" s="45"/>
-      <c r="BG37" s="45"/>
-      <c r="BH37" s="45"/>
-      <c r="BI37" s="45"/>
-      <c r="BJ37" s="1" t="s">
-        <v>63</v>
-      </c>
+      <c r="BF37" s="59"/>
+      <c r="BG37" s="59"/>
+      <c r="BH37" s="59"/>
+      <c r="BI37" s="59"/>
+      <c r="BJ37" s="1"/>
     </row>
     <row r="38" spans="1:62" ht="42" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
@@ -47926,6 +47938,9 @@
       </c>
       <c r="BI38" s="24" t="s">
         <v>126</v>
+      </c>
+      <c r="BJ38" s="66" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:62" x14ac:dyDescent="0.35">
@@ -53305,16 +53320,18 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE37:BI37"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="L37:P37"/>
+    <mergeCell ref="Q37:U37"/>
+    <mergeCell ref="V37:Z37"/>
+    <mergeCell ref="AA37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AT37"/>
+    <mergeCell ref="AU37:AY37"/>
+    <mergeCell ref="AZ37:BD37"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="G36:P36"/>
     <mergeCell ref="Q36:Z36"/>
@@ -53327,18 +53344,16 @@
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AU3:AY3"/>
     <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="BE37:BI37"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="L37:P37"/>
-    <mergeCell ref="Q37:U37"/>
-    <mergeCell ref="V37:Z37"/>
-    <mergeCell ref="AA37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AT37"/>
-    <mergeCell ref="AU37:AY37"/>
-    <mergeCell ref="AZ37:BD37"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53358,44 +53373,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44" t="s">
+      <c r="D1" s="58"/>
+      <c r="E1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44" t="s">
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44" t="s">
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="43" t="s">
+      <c r="R1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="57"/>
     </row>
     <row r="2" spans="1:20" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
@@ -55767,64 +55782,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -58276,34 +58291,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -60704,11 +60719,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60717,6 +60727,11 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60740,44 +60755,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -63250,44 +63265,44 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="49"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
@@ -65679,6 +65694,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -65686,13 +65708,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -65715,57 +65730,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="37"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
+      <c r="A1" s="51"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -68229,34 +68244,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -70654,17 +70669,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -70685,59 +70700,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="40"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -73245,34 +73260,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35" t="s">
+      <c r="D43" s="49"/>
+      <c r="E43" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="35"/>
-      <c r="G43" s="35"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35" t="s">
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="35"/>
-      <c r="L43" s="35"/>
-      <c r="M43" s="35"/>
-      <c r="N43" s="35" t="s">
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35"/>
-      <c r="Q43" s="35"/>
-      <c r="R43" s="34" t="s">
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="R43" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="34"/>
-      <c r="T43" s="34"/>
+      <c r="S43" s="48"/>
+      <c r="T43" s="48"/>
     </row>
     <row r="44" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -75667,17 +75682,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75701,57 +75716,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -78259,34 +78274,34 @@
       <c r="A44" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35" t="s">
+      <c r="D44" s="49"/>
+      <c r="E44" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="35"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35" t="s">
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35" t="s">
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="35"/>
-      <c r="P44" s="35"/>
-      <c r="Q44" s="35"/>
-      <c r="R44" s="34" t="s">
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="R44" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S44" s="34"/>
-      <c r="T44" s="34"/>
+      <c r="S44" s="48"/>
+      <c r="T44" s="48"/>
     </row>
     <row r="45" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
@@ -80935,17 +80950,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -80968,57 +80983,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="36"/>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -83480,34 +83495,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -85967,17 +85982,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -85998,24 +86013,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="41"/>
-      <c r="P1" s="41"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
@@ -86024,34 +86039,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -88497,34 +88512,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -90942,17 +90957,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -90976,34 +90991,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35" t="s">
+      <c r="D2" s="49"/>
+      <c r="E2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35" t="s">
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="34" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -93463,34 +93478,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35" t="s">
+      <c r="D42" s="49"/>
+      <c r="E42" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35" t="s">
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35" t="s">
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35"/>
-      <c r="Q42" s="35"/>
-      <c r="R42" s="34" t="s">
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="34"/>
-      <c r="T42" s="34"/>
+      <c r="S42" s="48"/>
+      <c r="T42" s="48"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -95947,16 +95962,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added column for display defautls
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5415FB8-6E42-4141-BC80-91252DE6A36B}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D2BADD6-258C-48C4-B1C8-F4DD7DCB6238}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="6" activeTab="17" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="155">
   <si>
     <t>State/UTs</t>
   </si>
@@ -517,6 +517,9 @@
   <si>
     <t>Equity_Categories</t>
   </si>
+  <si>
+    <t>Default_display</t>
+  </si>
 </sst>
 </file>
 
@@ -614,7 +617,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -690,60 +693,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -783,19 +732,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -813,21 +749,6 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -858,11 +779,134 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -951,20 +995,17 @@
       <alignment horizontal="right" vertical="top" indent="2" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1019,9 +1060,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1336,10 +1384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1347,329 +1395,396 @@
     <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="68" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="D1" s="70" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="35" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="46" t="str">
+      <c r="C2" s="61" t="str">
         <f>B2</f>
         <v>Any ANC</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="D2" s="67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F2" s="37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="36" t="str">
+      <c r="C3" s="62" t="str">
         <f t="shared" ref="C3:C17" si="0">B3</f>
         <v>ANC4+</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="D3" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="36" t="str">
+      <c r="C4" s="62" t="str">
         <f t="shared" si="0"/>
         <v>IFA for 100 days</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="D4" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="40" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="D5" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" s="37" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="36" t="str">
+      <c r="C6" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Institutional delivery</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="D6" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" s="37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="36" t="str">
+      <c r="C7" s="62" t="str">
         <f t="shared" si="0"/>
         <v>C-section delivery</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="D7" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="36" t="str">
+      <c r="C8" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Breastfeeding 1 hour</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="D8" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="37" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="36" t="str">
+      <c r="C9" s="62" t="str">
         <f t="shared" si="0"/>
         <v>PNC mother 2 days</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="D9" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F9" s="37" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="36" t="str">
+      <c r="C10" s="62" t="str">
         <f t="shared" si="0"/>
         <v>PNC children 2 days</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="D10" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F10" s="37" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="36" t="str">
+      <c r="C11" s="62" t="str">
         <f t="shared" si="0"/>
         <v>DPT3</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="D11" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="37" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="40" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="36" t="str">
+      <c r="C12" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Immunisation</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="D12" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="40" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="36" t="str">
+      <c r="C13" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Diarrhoea</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="D13" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13" s="37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="40" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="36" t="str">
+      <c r="C14" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Measles</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="D14" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F14" s="37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="40" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="36" t="str">
+      <c r="C15" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Stunted</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="D15" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F15" s="37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="40" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="36" t="str">
+      <c r="C16" s="62" t="str">
         <f t="shared" si="0"/>
         <v>Wasted</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="D16" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="37" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="40" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="43" t="str">
+      <c r="C17" s="63" t="str">
         <f t="shared" si="0"/>
         <v>Underweight</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="D17" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="D18" s="65" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" s="37" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B19" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="D19" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F19" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="D20" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="37" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="41" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="D21" s="65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F21" s="37" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="42" t="s">
+    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="D22" s="66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F22" s="38" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1696,65 +1811,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:26" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -4262,34 +4377,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49" t="s">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49" t="s">
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="48" t="s">
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
@@ -6793,57 +6908,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -9349,34 +9464,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49" t="s">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49" t="s">
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="48" t="s">
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AL43" s="2"/>
@@ -11821,17 +11936,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11853,59 +11968,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -14393,34 +14508,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49" t="s">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49" t="s">
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="48" t="s">
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -16850,17 +16965,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -16884,64 +16999,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -19399,34 +19514,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -21898,11 +22013,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -21911,6 +22021,11 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21933,44 +22048,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="56"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -24410,44 +24525,44 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A45" s="58" t="s">
+      <c r="A45" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="58"/>
-      <c r="E45" s="58" t="s">
+      <c r="D45" s="53"/>
+      <c r="E45" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
-      <c r="J45" s="58" t="s">
+      <c r="F45" s="53"/>
+      <c r="G45" s="53"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="58"/>
-      <c r="N45" s="58" t="s">
+      <c r="K45" s="53"/>
+      <c r="L45" s="53"/>
+      <c r="M45" s="53"/>
+      <c r="N45" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O45" s="58"/>
-      <c r="P45" s="58"/>
-      <c r="Q45" s="58"/>
-      <c r="R45" s="57" t="s">
+      <c r="O45" s="53"/>
+      <c r="P45" s="53"/>
+      <c r="Q45" s="53"/>
+      <c r="R45" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="57"/>
-      <c r="T45" s="57"/>
+      <c r="S45" s="52"/>
+      <c r="T45" s="52"/>
     </row>
     <row r="46" spans="1:26" ht="28" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="53"/>
+      <c r="B46" s="53"/>
       <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
@@ -26903,44 +27018,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="57" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -29384,44 +29499,44 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="58" t="s">
+      <c r="A42" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="58" t="s">
+      <c r="C42" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58" t="s">
+      <c r="D42" s="53"/>
+      <c r="E42" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58" t="s">
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K42" s="58"/>
-      <c r="L42" s="58"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58" t="s">
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="57" t="s">
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="57"/>
-      <c r="T42" s="57"/>
+      <c r="S42" s="52"/>
+      <c r="T42" s="52"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A43" s="58"/>
-      <c r="B43" s="58"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="53"/>
       <c r="C43" s="11" t="s">
         <v>7</v>
       </c>
@@ -31878,6 +31993,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -31885,13 +32007,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31909,44 +32024,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="57" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -34390,44 +34505,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="58" t="s">
+      <c r="A43" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58" t="s">
+      <c r="D43" s="53"/>
+      <c r="E43" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58" t="s">
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58" t="s">
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="57" t="s">
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="57"/>
-      <c r="T43" s="57"/>
+      <c r="S43" s="52"/>
+      <c r="T43" s="52"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -36884,6 +36999,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -36891,13 +37013,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36914,44 +37029,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58" t="s">
+      <c r="D2" s="53"/>
+      <c r="E2" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58" t="s">
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="58" t="s">
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="58"/>
-      <c r="P2" s="58"/>
-      <c r="Q2" s="58"/>
-      <c r="R2" s="57" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="58"/>
-      <c r="B3" s="58"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -39395,44 +39510,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="58" t="s">
+      <c r="A43" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="58"/>
-      <c r="E43" s="58" t="s">
+      <c r="D43" s="53"/>
+      <c r="E43" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58" t="s">
+      <c r="F43" s="53"/>
+      <c r="G43" s="53"/>
+      <c r="H43" s="53"/>
+      <c r="I43" s="53"/>
+      <c r="J43" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="58"/>
-      <c r="L43" s="58"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58" t="s">
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="57" t="s">
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="57"/>
-      <c r="T43" s="57"/>
+      <c r="S43" s="52"/>
+      <c r="T43" s="52"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="58"/>
-      <c r="B44" s="58"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -41889,6 +42004,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -41896,13 +42018,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -41912,8 +42027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX23" workbookViewId="0">
-      <selection activeCell="BJ38" sqref="BJ38"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -41930,157 +42045,157 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="60" t="s">
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="R2" s="61"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="61"/>
-      <c r="W2" s="61"/>
-      <c r="X2" s="61"/>
-      <c r="Y2" s="61"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="59" t="s">
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
+      <c r="Y2" s="56"/>
+      <c r="Z2" s="57"/>
+      <c r="AA2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="59"/>
-      <c r="AE2" s="59"/>
-      <c r="AF2" s="59"/>
-      <c r="AG2" s="59"/>
-      <c r="AH2" s="59"/>
-      <c r="AI2" s="59"/>
-      <c r="AJ2" s="59"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
       <c r="AK2" s="29"/>
       <c r="AL2" s="29"/>
       <c r="AM2" s="29"/>
       <c r="AN2" s="29"/>
-      <c r="AO2" s="63" t="s">
+      <c r="AO2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" s="64"/>
-      <c r="AQ2" s="64"/>
-      <c r="AR2" s="64"/>
-      <c r="AS2" s="64"/>
-      <c r="AT2" s="65"/>
+      <c r="AP2" s="59"/>
+      <c r="AQ2" s="59"/>
+      <c r="AR2" s="59"/>
+      <c r="AS2" s="59"/>
+      <c r="AT2" s="60"/>
       <c r="AU2" s="23"/>
       <c r="AV2" s="23"/>
       <c r="AW2" s="23"/>
       <c r="AX2" s="23"/>
-      <c r="AY2" s="59" t="s">
+      <c r="AY2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AZ2" s="59"/>
-      <c r="BA2" s="59"/>
-      <c r="BB2" s="59"/>
-      <c r="BC2" s="59"/>
-      <c r="BD2" s="59"/>
-      <c r="BE2" s="59"/>
-      <c r="BF2" s="59"/>
-      <c r="BG2" s="59"/>
-      <c r="BH2" s="59"/>
-      <c r="BI2" s="59"/>
+      <c r="AZ2" s="54"/>
+      <c r="BA2" s="54"/>
+      <c r="BB2" s="54"/>
+      <c r="BC2" s="54"/>
+      <c r="BD2" s="54"/>
+      <c r="BE2" s="54"/>
+      <c r="BF2" s="54"/>
+      <c r="BG2" s="54"/>
+      <c r="BH2" s="54"/>
+      <c r="BI2" s="54"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59" t="s">
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59" t="s">
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59" t="s">
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59" t="s">
+      <c r="R3" s="54"/>
+      <c r="S3" s="54"/>
+      <c r="T3" s="54"/>
+      <c r="U3" s="54"/>
+      <c r="V3" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
-      <c r="Y3" s="59"/>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="59" t="s">
+      <c r="W3" s="54"/>
+      <c r="X3" s="54"/>
+      <c r="Y3" s="54"/>
+      <c r="Z3" s="54"/>
+      <c r="AA3" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="59"/>
-      <c r="AC3" s="59"/>
-      <c r="AD3" s="59"/>
-      <c r="AE3" s="59"/>
-      <c r="AF3" s="59" t="s">
+      <c r="AB3" s="54"/>
+      <c r="AC3" s="54"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="54"/>
+      <c r="AF3" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="AG3" s="59"/>
-      <c r="AH3" s="59"/>
-      <c r="AI3" s="59"/>
-      <c r="AJ3" s="59"/>
-      <c r="AK3" s="59" t="s">
+      <c r="AG3" s="54"/>
+      <c r="AH3" s="54"/>
+      <c r="AI3" s="54"/>
+      <c r="AJ3" s="54"/>
+      <c r="AK3" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="59"/>
-      <c r="AM3" s="59"/>
-      <c r="AN3" s="59"/>
-      <c r="AO3" s="59"/>
-      <c r="AP3" s="59" t="s">
+      <c r="AL3" s="54"/>
+      <c r="AM3" s="54"/>
+      <c r="AN3" s="54"/>
+      <c r="AO3" s="54"/>
+      <c r="AP3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="59"/>
-      <c r="AR3" s="59"/>
-      <c r="AS3" s="59"/>
-      <c r="AT3" s="59"/>
-      <c r="AU3" s="59" t="s">
+      <c r="AQ3" s="54"/>
+      <c r="AR3" s="54"/>
+      <c r="AS3" s="54"/>
+      <c r="AT3" s="54"/>
+      <c r="AU3" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="59"/>
-      <c r="AW3" s="59"/>
-      <c r="AX3" s="59"/>
-      <c r="AY3" s="59"/>
-      <c r="AZ3" s="59" t="s">
+      <c r="AV3" s="54"/>
+      <c r="AW3" s="54"/>
+      <c r="AX3" s="54"/>
+      <c r="AY3" s="54"/>
+      <c r="AZ3" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="BA3" s="59"/>
-      <c r="BB3" s="59"/>
-      <c r="BC3" s="59"/>
-      <c r="BD3" s="59"/>
-      <c r="BE3" s="59" t="s">
+      <c r="BA3" s="54"/>
+      <c r="BB3" s="54"/>
+      <c r="BC3" s="54"/>
+      <c r="BD3" s="54"/>
+      <c r="BE3" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="59"/>
-      <c r="BG3" s="59"/>
-      <c r="BH3" s="59"/>
-      <c r="BI3" s="59"/>
+      <c r="BF3" s="54"/>
+      <c r="BG3" s="54"/>
+      <c r="BH3" s="54"/>
+      <c r="BI3" s="54"/>
       <c r="BJ3" s="1"/>
     </row>
     <row r="4" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -42265,7 +42380,7 @@
       <c r="BI4" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="BJ4" s="66" t="s">
+      <c r="BJ4" s="42" t="s">
         <v>63</v>
       </c>
     </row>
@@ -47601,160 +47716,160 @@
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="59" t="s">
+      <c r="G36" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="59"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="59"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="59"/>
-      <c r="N36" s="59"/>
-      <c r="O36" s="59"/>
-      <c r="P36" s="59"/>
-      <c r="Q36" s="60" t="s">
+      <c r="H36" s="54"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="54"/>
+      <c r="K36" s="54"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="54"/>
+      <c r="P36" s="54"/>
+      <c r="Q36" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="R36" s="61"/>
-      <c r="S36" s="61"/>
-      <c r="T36" s="61"/>
-      <c r="U36" s="61"/>
-      <c r="V36" s="61"/>
-      <c r="W36" s="61"/>
-      <c r="X36" s="61"/>
-      <c r="Y36" s="61"/>
-      <c r="Z36" s="62"/>
-      <c r="AA36" s="59" t="s">
+      <c r="R36" s="56"/>
+      <c r="S36" s="56"/>
+      <c r="T36" s="56"/>
+      <c r="U36" s="56"/>
+      <c r="V36" s="56"/>
+      <c r="W36" s="56"/>
+      <c r="X36" s="56"/>
+      <c r="Y36" s="56"/>
+      <c r="Z36" s="57"/>
+      <c r="AA36" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="AB36" s="59"/>
-      <c r="AC36" s="59"/>
-      <c r="AD36" s="59"/>
-      <c r="AE36" s="59"/>
-      <c r="AF36" s="59"/>
-      <c r="AG36" s="59"/>
-      <c r="AH36" s="59"/>
-      <c r="AI36" s="59"/>
-      <c r="AJ36" s="59"/>
+      <c r="AB36" s="54"/>
+      <c r="AC36" s="54"/>
+      <c r="AD36" s="54"/>
+      <c r="AE36" s="54"/>
+      <c r="AF36" s="54"/>
+      <c r="AG36" s="54"/>
+      <c r="AH36" s="54"/>
+      <c r="AI36" s="54"/>
+      <c r="AJ36" s="54"/>
       <c r="AK36" s="29"/>
       <c r="AL36" s="29"/>
       <c r="AM36" s="29"/>
       <c r="AN36" s="29"/>
-      <c r="AO36" s="63" t="s">
+      <c r="AO36" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="AP36" s="64"/>
-      <c r="AQ36" s="64"/>
-      <c r="AR36" s="64"/>
-      <c r="AS36" s="64"/>
-      <c r="AT36" s="65"/>
+      <c r="AP36" s="59"/>
+      <c r="AQ36" s="59"/>
+      <c r="AR36" s="59"/>
+      <c r="AS36" s="59"/>
+      <c r="AT36" s="60"/>
       <c r="AU36" s="23"/>
       <c r="AV36" s="23"/>
       <c r="AW36" s="23"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="59" t="s">
+      <c r="AY36" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AZ36" s="59"/>
-      <c r="BA36" s="59"/>
-      <c r="BB36" s="59"/>
-      <c r="BC36" s="59"/>
-      <c r="BD36" s="59"/>
-      <c r="BE36" s="59"/>
-      <c r="BF36" s="59"/>
-      <c r="BG36" s="59"/>
-      <c r="BH36" s="59"/>
-      <c r="BI36" s="59"/>
+      <c r="AZ36" s="54"/>
+      <c r="BA36" s="54"/>
+      <c r="BB36" s="54"/>
+      <c r="BC36" s="54"/>
+      <c r="BD36" s="54"/>
+      <c r="BE36" s="54"/>
+      <c r="BF36" s="54"/>
+      <c r="BG36" s="54"/>
+      <c r="BH36" s="54"/>
+      <c r="BI36" s="54"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59" t="s">
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59" t="s">
+      <c r="H37" s="54"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="54"/>
+      <c r="K37" s="54"/>
+      <c r="L37" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="59"/>
-      <c r="N37" s="59"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="59"/>
-      <c r="Q37" s="59" t="s">
+      <c r="M37" s="54"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="54"/>
+      <c r="P37" s="54"/>
+      <c r="Q37" s="54" t="s">
         <v>120</v>
       </c>
-      <c r="R37" s="59"/>
-      <c r="S37" s="59"/>
-      <c r="T37" s="59"/>
-      <c r="U37" s="59"/>
-      <c r="V37" s="59" t="s">
+      <c r="R37" s="54"/>
+      <c r="S37" s="54"/>
+      <c r="T37" s="54"/>
+      <c r="U37" s="54"/>
+      <c r="V37" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="W37" s="59"/>
-      <c r="X37" s="59"/>
-      <c r="Y37" s="59"/>
-      <c r="Z37" s="59"/>
-      <c r="AA37" s="59" t="s">
+      <c r="W37" s="54"/>
+      <c r="X37" s="54"/>
+      <c r="Y37" s="54"/>
+      <c r="Z37" s="54"/>
+      <c r="AA37" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="AB37" s="59"/>
-      <c r="AC37" s="59"/>
-      <c r="AD37" s="59"/>
-      <c r="AE37" s="59"/>
-      <c r="AF37" s="59" t="s">
+      <c r="AB37" s="54"/>
+      <c r="AC37" s="54"/>
+      <c r="AD37" s="54"/>
+      <c r="AE37" s="54"/>
+      <c r="AF37" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="AG37" s="59"/>
-      <c r="AH37" s="59"/>
-      <c r="AI37" s="59"/>
-      <c r="AJ37" s="59"/>
-      <c r="AK37" s="59" t="s">
+      <c r="AG37" s="54"/>
+      <c r="AH37" s="54"/>
+      <c r="AI37" s="54"/>
+      <c r="AJ37" s="54"/>
+      <c r="AK37" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="AL37" s="59"/>
-      <c r="AM37" s="59"/>
-      <c r="AN37" s="59"/>
-      <c r="AO37" s="59"/>
-      <c r="AP37" s="59" t="s">
+      <c r="AL37" s="54"/>
+      <c r="AM37" s="54"/>
+      <c r="AN37" s="54"/>
+      <c r="AO37" s="54"/>
+      <c r="AP37" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="AQ37" s="59"/>
-      <c r="AR37" s="59"/>
-      <c r="AS37" s="59"/>
-      <c r="AT37" s="59"/>
-      <c r="AU37" s="59" t="s">
+      <c r="AQ37" s="54"/>
+      <c r="AR37" s="54"/>
+      <c r="AS37" s="54"/>
+      <c r="AT37" s="54"/>
+      <c r="AU37" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="AV37" s="59"/>
-      <c r="AW37" s="59"/>
-      <c r="AX37" s="59"/>
-      <c r="AY37" s="59"/>
-      <c r="AZ37" s="59" t="s">
+      <c r="AV37" s="54"/>
+      <c r="AW37" s="54"/>
+      <c r="AX37" s="54"/>
+      <c r="AY37" s="54"/>
+      <c r="AZ37" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="BA37" s="59"/>
-      <c r="BB37" s="59"/>
-      <c r="BC37" s="59"/>
-      <c r="BD37" s="59"/>
-      <c r="BE37" s="59" t="s">
+      <c r="BA37" s="54"/>
+      <c r="BB37" s="54"/>
+      <c r="BC37" s="54"/>
+      <c r="BD37" s="54"/>
+      <c r="BE37" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="BF37" s="59"/>
-      <c r="BG37" s="59"/>
-      <c r="BH37" s="59"/>
-      <c r="BI37" s="59"/>
+      <c r="BF37" s="54"/>
+      <c r="BG37" s="54"/>
+      <c r="BH37" s="54"/>
+      <c r="BI37" s="54"/>
       <c r="BJ37" s="1"/>
     </row>
     <row r="38" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -47939,7 +48054,7 @@
       <c r="BI38" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="BJ38" s="66" t="s">
+      <c r="BJ38" s="42" t="s">
         <v>63</v>
       </c>
     </row>
@@ -53320,6 +53435,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="G36:P36"/>
+    <mergeCell ref="Q36:Z36"/>
+    <mergeCell ref="AA36:AJ36"/>
+    <mergeCell ref="AO36:AT36"/>
+    <mergeCell ref="AY36:BI36"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="AZ3:BD3"/>
     <mergeCell ref="BE37:BI37"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="G37:K37"/>
@@ -53332,28 +53469,6 @@
     <mergeCell ref="AP37:AT37"/>
     <mergeCell ref="AU37:AY37"/>
     <mergeCell ref="AZ37:BD37"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="G36:P36"/>
-    <mergeCell ref="Q36:Z36"/>
-    <mergeCell ref="AA36:AJ36"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AY36:BI36"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AU3:AY3"/>
-    <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53373,44 +53488,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58" t="s">
+      <c r="D1" s="53"/>
+      <c r="E1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58" t="s">
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="57" t="s">
+      <c r="R1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="57"/>
-      <c r="T1" s="57"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
     </row>
     <row r="2" spans="1:20" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
@@ -55782,64 +55897,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -58291,34 +58406,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -60719,6 +60834,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60727,11 +60847,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60755,44 +60870,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="49"/>
-      <c r="B3" s="49"/>
+      <c r="A3" s="44"/>
+      <c r="B3" s="44"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -63265,44 +63380,44 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="49" t="s">
+      <c r="A42" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A43" s="49"/>
-      <c r="B43" s="49"/>
+      <c r="A43" s="44"/>
+      <c r="B43" s="44"/>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
@@ -65694,6 +65809,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -65701,13 +65823,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -65730,57 +65845,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="51"/>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -68244,34 +68359,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -70669,17 +70784,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -70700,59 +70815,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -73260,34 +73375,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="49" t="s">
+      <c r="C43" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49" t="s">
+      <c r="D43" s="44"/>
+      <c r="E43" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49" t="s">
+      <c r="F43" s="44"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="44"/>
+      <c r="I43" s="44"/>
+      <c r="J43" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49" t="s">
+      <c r="K43" s="44"/>
+      <c r="L43" s="44"/>
+      <c r="M43" s="44"/>
+      <c r="N43" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="R43" s="48" t="s">
+      <c r="O43" s="44"/>
+      <c r="P43" s="44"/>
+      <c r="Q43" s="44"/>
+      <c r="R43" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="48"/>
-      <c r="T43" s="48"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
     </row>
     <row r="44" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -75682,17 +75797,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75716,57 +75831,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -78274,34 +78389,34 @@
       <c r="A44" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49" t="s">
+      <c r="D44" s="44"/>
+      <c r="E44" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="49" t="s">
+      <c r="F44" s="44"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="44"/>
+      <c r="I44" s="44"/>
+      <c r="J44" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49" t="s">
+      <c r="K44" s="44"/>
+      <c r="L44" s="44"/>
+      <c r="M44" s="44"/>
+      <c r="N44" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="49"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="49"/>
-      <c r="R44" s="48" t="s">
+      <c r="O44" s="44"/>
+      <c r="P44" s="44"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S44" s="48"/>
-      <c r="T44" s="48"/>
+      <c r="S44" s="43"/>
+      <c r="T44" s="43"/>
     </row>
     <row r="45" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
@@ -80950,17 +81065,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -80983,57 +81098,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -83495,34 +83610,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -85982,17 +86097,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -86013,24 +86128,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
@@ -86039,34 +86154,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -88512,34 +88627,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -90957,17 +91072,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -90991,34 +91106,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49" t="s">
+      <c r="D2" s="44"/>
+      <c r="E2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="48" t="s">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -93478,34 +93593,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49" t="s">
+      <c r="D42" s="44"/>
+      <c r="E42" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="49" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="44"/>
+      <c r="I42" s="44"/>
+      <c r="J42" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49" t="s">
+      <c r="K42" s="44"/>
+      <c r="L42" s="44"/>
+      <c r="M42" s="44"/>
+      <c r="N42" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="48" t="s">
+      <c r="O42" s="44"/>
+      <c r="P42" s="44"/>
+      <c r="Q42" s="44"/>
+      <c r="R42" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="48"/>
-      <c r="T42" s="48"/>
+      <c r="S42" s="43"/>
+      <c r="T42" s="43"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -95962,16 +96077,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added disaggregation domains and defaults for equity table from excel template
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D2BADD6-258C-48C4-B1C8-F4DD7DCB6238}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6F829A4-AA21-4E60-882E-B0C2C0726779}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3607" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3631" uniqueCount="162">
   <si>
     <t>State/UTs</t>
   </si>
@@ -520,6 +520,27 @@
   <si>
     <t>Default_display</t>
   </si>
+  <si>
+    <t>Equity_Domains</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>Wealth</t>
+  </si>
+  <si>
+    <t>Women's Education</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Default_Cat_A</t>
+  </si>
+  <si>
+    <t>Default_Cat_B</t>
+  </si>
 </sst>
 </file>
 
@@ -617,7 +638,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -902,11 +923,128 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1006,6 +1144,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1060,16 +1208,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1384,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F1" sqref="F1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1396,396 +1544,597 @@
     <col min="2" max="2" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="51" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="50" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="51" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H1" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" s="72" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="39" t="s">
         <v>147</v>
       </c>
       <c r="B2" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="61" t="str">
+      <c r="C2" s="43" t="str">
         <f>B2</f>
         <v>Any ANC</v>
       </c>
-      <c r="D2" s="67" t="b">
+      <c r="D2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="73" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="71" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
         <v>147</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="C3" s="62" t="str">
+      <c r="C3" s="44" t="str">
         <f t="shared" ref="C3:C17" si="0">B3</f>
         <v>ANC4+</v>
       </c>
-      <c r="D3" s="65" t="b">
+      <c r="D3" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="G3" s="71" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H3" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
         <v>147</v>
       </c>
       <c r="B4" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="C4" s="62" t="str">
+      <c r="C4" s="44" t="str">
         <f t="shared" si="0"/>
         <v>IFA for 100 days</v>
       </c>
-      <c r="D4" s="65" t="b">
+      <c r="D4" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="75" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="44" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H4" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
         <v>147</v>
       </c>
       <c r="B5" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="D5" s="65" t="b">
+      <c r="D5" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="77" t="s">
+        <v>157</v>
+      </c>
+      <c r="G5" s="44" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H5" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
         <v>149</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="62" t="str">
+      <c r="C6" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Institutional delivery</v>
       </c>
-      <c r="D6" s="65" t="b">
+      <c r="D6" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="44" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H6" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
         <v>149</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="62" t="str">
+      <c r="C7" s="44" t="str">
         <f t="shared" si="0"/>
         <v>C-section delivery</v>
       </c>
-      <c r="D7" s="65" t="b">
+      <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H7" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
         <v>150</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="62" t="str">
+      <c r="C8" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Breastfeeding 1 hour</v>
       </c>
-      <c r="D8" s="65" t="b">
+      <c r="D8" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H8" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
         <v>150</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="C9" s="62" t="str">
+      <c r="C9" s="44" t="str">
         <f t="shared" si="0"/>
         <v>PNC mother 2 days</v>
       </c>
-      <c r="D9" s="65" t="b">
+      <c r="D9" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="78" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="44" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H9" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="36" t="s">
         <v>150</v>
       </c>
       <c r="B10" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="C10" s="62" t="str">
+      <c r="C10" s="44" t="str">
         <f t="shared" si="0"/>
         <v>PNC children 2 days</v>
       </c>
-      <c r="D10" s="65" t="b">
+      <c r="D10" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="77" t="s">
+        <v>158</v>
+      </c>
+      <c r="G10" s="44" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H10" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="36" t="s">
         <v>151</v>
       </c>
       <c r="B11" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="62" t="str">
+      <c r="C11" s="44" t="str">
         <f t="shared" si="0"/>
         <v>DPT3</v>
       </c>
-      <c r="D11" s="65" t="b">
+      <c r="D11" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="G11" s="44" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H11" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="36" t="s">
         <v>151</v>
       </c>
       <c r="B12" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="62" t="str">
+      <c r="C12" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Immunisation</v>
       </c>
-      <c r="D12" s="65" t="b">
+      <c r="D12" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="G12" s="44" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H12" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="36" t="s">
         <v>152</v>
       </c>
       <c r="B13" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="62" t="str">
+      <c r="C13" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Diarrhoea</v>
       </c>
-      <c r="D13" s="65" t="b">
+      <c r="D13" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="78" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13" s="44" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H13" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
         <v>151</v>
       </c>
       <c r="B14" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="62" t="str">
+      <c r="C14" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Measles</v>
       </c>
-      <c r="D14" s="65" t="b">
+      <c r="D14" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="44" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H14" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="36" t="s">
         <v>152</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="62" t="str">
+      <c r="C15" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Stunted</v>
       </c>
-      <c r="D15" s="65" t="b">
+      <c r="D15" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="44" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H15" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="36" t="s">
         <v>152</v>
       </c>
       <c r="B16" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="62" t="str">
+      <c r="C16" s="44" t="str">
         <f t="shared" si="0"/>
         <v>Wasted</v>
       </c>
-      <c r="D16" s="65" t="b">
+      <c r="D16" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="44" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H16" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="36" t="s">
         <v>152</v>
       </c>
       <c r="B17" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="63" t="str">
+      <c r="C17" s="45" t="str">
         <f t="shared" si="0"/>
         <v>Underweight</v>
       </c>
-      <c r="D17" s="65" t="b">
+      <c r="D17" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="44" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H17" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B18" t="s">
         <v>125</v>
       </c>
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="65" t="b">
+      <c r="D18" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="77" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H18" s="44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B19" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D19" s="65" t="b">
+      <c r="D19" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H19" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B20" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="62" t="s">
+      <c r="C20" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="65" t="b">
+      <c r="D20" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="44" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H20" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="62" t="s">
+      <c r="C21" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="D21" s="65" t="b">
+      <c r="D21" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="G21" s="44" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H21" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="38" t="s">
         <v>125</v>
       </c>
       <c r="B22" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="64" t="s">
+      <c r="C22" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="66" t="b">
+      <c r="D22" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F22" s="79" t="s">
+        <v>159</v>
+      </c>
+      <c r="G22" s="46" t="s">
         <v>120</v>
+      </c>
+      <c r="H22" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="80" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1811,65 +2160,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
-      <c r="U1" s="45"/>
-      <c r="V1" s="45"/>
-      <c r="W1" s="45"/>
-      <c r="X1" s="45"/>
-      <c r="Y1" s="45"/>
-      <c r="Z1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:26" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -4377,34 +4726,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="54"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
@@ -6908,57 +7257,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -9464,34 +9813,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="54"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AL43" s="2"/>
@@ -11936,17 +12285,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11968,59 +12317,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="T1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -14508,34 +14857,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="54"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -16965,17 +17314,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -16999,64 +17348,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -19514,34 +19863,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -22013,6 +22362,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -22021,11 +22375,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22048,44 +22397,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="51"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="61"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -24525,44 +24874,44 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="53" t="s">
+      <c r="B45" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53" t="s">
+      <c r="D45" s="63"/>
+      <c r="E45" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53" t="s">
+      <c r="F45" s="63"/>
+      <c r="G45" s="63"/>
+      <c r="H45" s="63"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="53"/>
-      <c r="L45" s="53"/>
-      <c r="M45" s="53"/>
-      <c r="N45" s="53" t="s">
+      <c r="K45" s="63"/>
+      <c r="L45" s="63"/>
+      <c r="M45" s="63"/>
+      <c r="N45" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O45" s="53"/>
-      <c r="P45" s="53"/>
-      <c r="Q45" s="53"/>
-      <c r="R45" s="52" t="s">
+      <c r="O45" s="63"/>
+      <c r="P45" s="63"/>
+      <c r="Q45" s="63"/>
+      <c r="R45" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="52"/>
-      <c r="T45" s="52"/>
+      <c r="S45" s="62"/>
+      <c r="T45" s="62"/>
     </row>
     <row r="46" spans="1:26" ht="28" x14ac:dyDescent="0.35">
-      <c r="A46" s="53"/>
-      <c r="B46" s="53"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
@@ -27018,44 +27367,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="52" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -29499,44 +29848,44 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="53" t="s">
+      <c r="A42" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="53" t="s">
+      <c r="B42" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="53" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="53"/>
-      <c r="E42" s="53" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="52" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="52"/>
-      <c r="T42" s="52"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A43" s="53"/>
-      <c r="B43" s="53"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
       <c r="C43" s="11" t="s">
         <v>7</v>
       </c>
@@ -31993,6 +32342,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -32000,13 +32356,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32024,44 +32373,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="52" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -34505,44 +34854,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="52" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -36999,6 +37348,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -37006,13 +37362,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37029,44 +37378,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="52" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="53"/>
-      <c r="B3" s="53"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -39510,44 +39859,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="53" t="s">
+      <c r="A43" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="53" t="s">
+      <c r="B43" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="53" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="53"/>
-      <c r="H43" s="53"/>
-      <c r="I43" s="53"/>
-      <c r="J43" s="53" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="53"/>
-      <c r="L43" s="53"/>
-      <c r="M43" s="53"/>
-      <c r="N43" s="53" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="53"/>
-      <c r="P43" s="53"/>
-      <c r="Q43" s="53"/>
-      <c r="R43" s="52" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="52"/>
-      <c r="T43" s="52"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="63"/>
+      <c r="B44" s="63"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -42004,6 +42353,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -42011,13 +42367,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42045,157 +42394,157 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="55" t="s">
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="57"/>
-      <c r="AA2" s="54" t="s">
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="66"/>
+      <c r="V2" s="66"/>
+      <c r="W2" s="66"/>
+      <c r="X2" s="66"/>
+      <c r="Y2" s="66"/>
+      <c r="Z2" s="67"/>
+      <c r="AA2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
+      <c r="AB2" s="64"/>
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AG2" s="64"/>
+      <c r="AH2" s="64"/>
+      <c r="AI2" s="64"/>
+      <c r="AJ2" s="64"/>
       <c r="AK2" s="29"/>
       <c r="AL2" s="29"/>
       <c r="AM2" s="29"/>
       <c r="AN2" s="29"/>
-      <c r="AO2" s="58" t="s">
+      <c r="AO2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" s="59"/>
-      <c r="AQ2" s="59"/>
-      <c r="AR2" s="59"/>
-      <c r="AS2" s="59"/>
-      <c r="AT2" s="60"/>
+      <c r="AP2" s="69"/>
+      <c r="AQ2" s="69"/>
+      <c r="AR2" s="69"/>
+      <c r="AS2" s="69"/>
+      <c r="AT2" s="70"/>
       <c r="AU2" s="23"/>
       <c r="AV2" s="23"/>
       <c r="AW2" s="23"/>
       <c r="AX2" s="23"/>
-      <c r="AY2" s="54" t="s">
+      <c r="AY2" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="AZ2" s="54"/>
-      <c r="BA2" s="54"/>
-      <c r="BB2" s="54"/>
-      <c r="BC2" s="54"/>
-      <c r="BD2" s="54"/>
-      <c r="BE2" s="54"/>
-      <c r="BF2" s="54"/>
-      <c r="BG2" s="54"/>
-      <c r="BH2" s="54"/>
-      <c r="BI2" s="54"/>
+      <c r="AZ2" s="64"/>
+      <c r="BA2" s="64"/>
+      <c r="BB2" s="64"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="64"/>
+      <c r="BF2" s="64"/>
+      <c r="BG2" s="64"/>
+      <c r="BH2" s="64"/>
+      <c r="BI2" s="64"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54" t="s">
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54" t="s">
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54" t="s">
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54" t="s">
+      <c r="R3" s="64"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="64"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54" t="s">
+      <c r="W3" s="64"/>
+      <c r="X3" s="64"/>
+      <c r="Y3" s="64"/>
+      <c r="Z3" s="64"/>
+      <c r="AA3" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54" t="s">
+      <c r="AB3" s="64"/>
+      <c r="AC3" s="64"/>
+      <c r="AD3" s="64"/>
+      <c r="AE3" s="64"/>
+      <c r="AF3" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54" t="s">
+      <c r="AG3" s="64"/>
+      <c r="AH3" s="64"/>
+      <c r="AI3" s="64"/>
+      <c r="AJ3" s="64"/>
+      <c r="AK3" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="54"/>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54" t="s">
+      <c r="AL3" s="64"/>
+      <c r="AM3" s="64"/>
+      <c r="AN3" s="64"/>
+      <c r="AO3" s="64"/>
+      <c r="AP3" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="54"/>
-      <c r="AS3" s="54"/>
-      <c r="AT3" s="54"/>
-      <c r="AU3" s="54" t="s">
+      <c r="AQ3" s="64"/>
+      <c r="AR3" s="64"/>
+      <c r="AS3" s="64"/>
+      <c r="AT3" s="64"/>
+      <c r="AU3" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="54"/>
-      <c r="AW3" s="54"/>
-      <c r="AX3" s="54"/>
-      <c r="AY3" s="54"/>
-      <c r="AZ3" s="54" t="s">
+      <c r="AV3" s="64"/>
+      <c r="AW3" s="64"/>
+      <c r="AX3" s="64"/>
+      <c r="AY3" s="64"/>
+      <c r="AZ3" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BA3" s="54"/>
-      <c r="BB3" s="54"/>
-      <c r="BC3" s="54"/>
-      <c r="BD3" s="54"/>
-      <c r="BE3" s="54" t="s">
+      <c r="BA3" s="64"/>
+      <c r="BB3" s="64"/>
+      <c r="BC3" s="64"/>
+      <c r="BD3" s="64"/>
+      <c r="BE3" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="54"/>
-      <c r="BG3" s="54"/>
-      <c r="BH3" s="54"/>
-      <c r="BI3" s="54"/>
+      <c r="BF3" s="64"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="64"/>
+      <c r="BI3" s="64"/>
       <c r="BJ3" s="1"/>
     </row>
     <row r="4" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -47716,160 +48065,160 @@
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="54" t="s">
+      <c r="G36" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
-      <c r="O36" s="54"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="55" t="s">
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="64"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="64"/>
+      <c r="P36" s="64"/>
+      <c r="Q36" s="65" t="s">
         <v>119</v>
       </c>
-      <c r="R36" s="56"/>
-      <c r="S36" s="56"/>
-      <c r="T36" s="56"/>
-      <c r="U36" s="56"/>
-      <c r="V36" s="56"/>
-      <c r="W36" s="56"/>
-      <c r="X36" s="56"/>
-      <c r="Y36" s="56"/>
-      <c r="Z36" s="57"/>
-      <c r="AA36" s="54" t="s">
+      <c r="R36" s="66"/>
+      <c r="S36" s="66"/>
+      <c r="T36" s="66"/>
+      <c r="U36" s="66"/>
+      <c r="V36" s="66"/>
+      <c r="W36" s="66"/>
+      <c r="X36" s="66"/>
+      <c r="Y36" s="66"/>
+      <c r="Z36" s="67"/>
+      <c r="AA36" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="AB36" s="54"/>
-      <c r="AC36" s="54"/>
-      <c r="AD36" s="54"/>
-      <c r="AE36" s="54"/>
-      <c r="AF36" s="54"/>
-      <c r="AG36" s="54"/>
-      <c r="AH36" s="54"/>
-      <c r="AI36" s="54"/>
-      <c r="AJ36" s="54"/>
+      <c r="AB36" s="64"/>
+      <c r="AC36" s="64"/>
+      <c r="AD36" s="64"/>
+      <c r="AE36" s="64"/>
+      <c r="AF36" s="64"/>
+      <c r="AG36" s="64"/>
+      <c r="AH36" s="64"/>
+      <c r="AI36" s="64"/>
+      <c r="AJ36" s="64"/>
       <c r="AK36" s="29"/>
       <c r="AL36" s="29"/>
       <c r="AM36" s="29"/>
       <c r="AN36" s="29"/>
-      <c r="AO36" s="58" t="s">
+      <c r="AO36" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="AP36" s="59"/>
-      <c r="AQ36" s="59"/>
-      <c r="AR36" s="59"/>
-      <c r="AS36" s="59"/>
-      <c r="AT36" s="60"/>
+      <c r="AP36" s="69"/>
+      <c r="AQ36" s="69"/>
+      <c r="AR36" s="69"/>
+      <c r="AS36" s="69"/>
+      <c r="AT36" s="70"/>
       <c r="AU36" s="23"/>
       <c r="AV36" s="23"/>
       <c r="AW36" s="23"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="54" t="s">
+      <c r="AY36" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="AZ36" s="54"/>
-      <c r="BA36" s="54"/>
-      <c r="BB36" s="54"/>
-      <c r="BC36" s="54"/>
-      <c r="BD36" s="54"/>
-      <c r="BE36" s="54"/>
-      <c r="BF36" s="54"/>
-      <c r="BG36" s="54"/>
-      <c r="BH36" s="54"/>
-      <c r="BI36" s="54"/>
+      <c r="AZ36" s="64"/>
+      <c r="BA36" s="64"/>
+      <c r="BB36" s="64"/>
+      <c r="BC36" s="64"/>
+      <c r="BD36" s="64"/>
+      <c r="BE36" s="64"/>
+      <c r="BF36" s="64"/>
+      <c r="BG36" s="64"/>
+      <c r="BH36" s="64"/>
+      <c r="BI36" s="64"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="54" t="s">
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="54"/>
-      <c r="I37" s="54"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="54"/>
-      <c r="L37" s="54" t="s">
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="64"/>
+      <c r="L37" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="54"/>
-      <c r="N37" s="54"/>
-      <c r="O37" s="54"/>
-      <c r="P37" s="54"/>
-      <c r="Q37" s="54" t="s">
+      <c r="M37" s="64"/>
+      <c r="N37" s="64"/>
+      <c r="O37" s="64"/>
+      <c r="P37" s="64"/>
+      <c r="Q37" s="64" t="s">
         <v>120</v>
       </c>
-      <c r="R37" s="54"/>
-      <c r="S37" s="54"/>
-      <c r="T37" s="54"/>
-      <c r="U37" s="54"/>
-      <c r="V37" s="54" t="s">
+      <c r="R37" s="64"/>
+      <c r="S37" s="64"/>
+      <c r="T37" s="64"/>
+      <c r="U37" s="64"/>
+      <c r="V37" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="W37" s="54"/>
-      <c r="X37" s="54"/>
-      <c r="Y37" s="54"/>
-      <c r="Z37" s="54"/>
-      <c r="AA37" s="54" t="s">
+      <c r="W37" s="64"/>
+      <c r="X37" s="64"/>
+      <c r="Y37" s="64"/>
+      <c r="Z37" s="64"/>
+      <c r="AA37" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="AB37" s="54"/>
-      <c r="AC37" s="54"/>
-      <c r="AD37" s="54"/>
-      <c r="AE37" s="54"/>
-      <c r="AF37" s="54" t="s">
+      <c r="AB37" s="64"/>
+      <c r="AC37" s="64"/>
+      <c r="AD37" s="64"/>
+      <c r="AE37" s="64"/>
+      <c r="AF37" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="AG37" s="54"/>
-      <c r="AH37" s="54"/>
-      <c r="AI37" s="54"/>
-      <c r="AJ37" s="54"/>
-      <c r="AK37" s="54" t="s">
+      <c r="AG37" s="64"/>
+      <c r="AH37" s="64"/>
+      <c r="AI37" s="64"/>
+      <c r="AJ37" s="64"/>
+      <c r="AK37" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="AL37" s="54"/>
-      <c r="AM37" s="54"/>
-      <c r="AN37" s="54"/>
-      <c r="AO37" s="54"/>
-      <c r="AP37" s="54" t="s">
+      <c r="AL37" s="64"/>
+      <c r="AM37" s="64"/>
+      <c r="AN37" s="64"/>
+      <c r="AO37" s="64"/>
+      <c r="AP37" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="AQ37" s="54"/>
-      <c r="AR37" s="54"/>
-      <c r="AS37" s="54"/>
-      <c r="AT37" s="54"/>
-      <c r="AU37" s="54" t="s">
+      <c r="AQ37" s="64"/>
+      <c r="AR37" s="64"/>
+      <c r="AS37" s="64"/>
+      <c r="AT37" s="64"/>
+      <c r="AU37" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="AV37" s="54"/>
-      <c r="AW37" s="54"/>
-      <c r="AX37" s="54"/>
-      <c r="AY37" s="54"/>
-      <c r="AZ37" s="54" t="s">
+      <c r="AV37" s="64"/>
+      <c r="AW37" s="64"/>
+      <c r="AX37" s="64"/>
+      <c r="AY37" s="64"/>
+      <c r="AZ37" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BA37" s="54"/>
-      <c r="BB37" s="54"/>
-      <c r="BC37" s="54"/>
-      <c r="BD37" s="54"/>
-      <c r="BE37" s="54" t="s">
+      <c r="BA37" s="64"/>
+      <c r="BB37" s="64"/>
+      <c r="BC37" s="64"/>
+      <c r="BD37" s="64"/>
+      <c r="BE37" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="BF37" s="54"/>
-      <c r="BG37" s="54"/>
-      <c r="BH37" s="54"/>
-      <c r="BI37" s="54"/>
+      <c r="BF37" s="64"/>
+      <c r="BG37" s="64"/>
+      <c r="BH37" s="64"/>
+      <c r="BI37" s="64"/>
       <c r="BJ37" s="1"/>
     </row>
     <row r="38" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -53435,16 +53784,18 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE37:BI37"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="L37:P37"/>
+    <mergeCell ref="Q37:U37"/>
+    <mergeCell ref="V37:Z37"/>
+    <mergeCell ref="AA37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AT37"/>
+    <mergeCell ref="AU37:AY37"/>
+    <mergeCell ref="AZ37:BD37"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="G36:P36"/>
     <mergeCell ref="Q36:Z36"/>
@@ -53457,18 +53808,16 @@
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AU3:AY3"/>
     <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="BE37:BI37"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="L37:P37"/>
-    <mergeCell ref="Q37:U37"/>
-    <mergeCell ref="V37:Z37"/>
-    <mergeCell ref="AA37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AT37"/>
-    <mergeCell ref="AU37:AY37"/>
-    <mergeCell ref="AZ37:BD37"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53488,44 +53837,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53" t="s">
+      <c r="D1" s="63"/>
+      <c r="E1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53" t="s">
+      <c r="K1" s="63"/>
+      <c r="L1" s="63"/>
+      <c r="M1" s="63"/>
+      <c r="N1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="O1" s="63"/>
+      <c r="P1" s="63"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="52"/>
-      <c r="T1" s="52"/>
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
     </row>
     <row r="2" spans="1:20" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
+      <c r="A2" s="63"/>
+      <c r="B2" s="63"/>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
@@ -55897,64 +56246,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -58406,34 +58755,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -60834,11 +61183,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -60847,6 +61191,11 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -60870,44 +61219,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="44"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -63380,44 +63729,44 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A43" s="44"/>
-      <c r="B43" s="44"/>
+      <c r="A43" s="54"/>
+      <c r="B43" s="54"/>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
@@ -65809,6 +66158,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -65816,13 +66172,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -65845,57 +66194,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="46"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
+      <c r="A1" s="56"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -68359,34 +68708,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -70784,17 +71133,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -70815,59 +71164,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -73375,34 +73724,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="44"/>
-      <c r="E43" s="44" t="s">
+      <c r="D43" s="54"/>
+      <c r="E43" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44" t="s">
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="44"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="44"/>
-      <c r="N43" s="44" t="s">
+      <c r="K43" s="54"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="54"/>
+      <c r="N43" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="44"/>
-      <c r="Q43" s="44"/>
-      <c r="R43" s="43" t="s">
+      <c r="O43" s="54"/>
+      <c r="P43" s="54"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
     </row>
     <row r="44" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -75797,17 +76146,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75831,57 +76180,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -78389,34 +78738,34 @@
       <c r="A44" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="44" t="s">
+      <c r="C44" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="44"/>
-      <c r="E44" s="44" t="s">
+      <c r="D44" s="54"/>
+      <c r="E44" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44" t="s">
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K44" s="44"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="44"/>
-      <c r="N44" s="44" t="s">
+      <c r="K44" s="54"/>
+      <c r="L44" s="54"/>
+      <c r="M44" s="54"/>
+      <c r="N44" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="44"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="44"/>
-      <c r="R44" s="43" t="s">
+      <c r="O44" s="54"/>
+      <c r="P44" s="54"/>
+      <c r="Q44" s="54"/>
+      <c r="R44" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S44" s="43"/>
-      <c r="T44" s="43"/>
+      <c r="S44" s="53"/>
+      <c r="T44" s="53"/>
     </row>
     <row r="45" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
@@ -81065,17 +81414,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -81098,57 +81447,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="45"/>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-      <c r="O1" s="45"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45"/>
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -83610,34 +83959,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -86097,17 +86446,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -86128,24 +86477,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
+      <c r="A1" s="60"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
@@ -86154,34 +86503,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -88627,34 +88976,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -91072,17 +91421,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -91106,34 +91455,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="D2" s="54"/>
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44" t="s">
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="43" t="s">
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -93593,34 +93942,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="44" t="s">
+      <c r="C42" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="54"/>
+      <c r="E42" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="44"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44" t="s">
+      <c r="F42" s="54"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="44"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="44"/>
-      <c r="N42" s="44" t="s">
+      <c r="K42" s="54"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="54"/>
+      <c r="N42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="44"/>
-      <c r="Q42" s="44"/>
-      <c r="R42" s="43" t="s">
+      <c r="O42" s="54"/>
+      <c r="P42" s="54"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="43"/>
-      <c r="T42" s="43"/>
+      <c r="S42" s="53"/>
+      <c r="T42" s="53"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -96077,16 +96426,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
corrected child mortality india nhfs 4
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6F829A4-AA21-4E60-882E-B0C2C0726779}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9794DDE4-6943-4539-9269-61CDC836FDC6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Wasted" sheetId="22" r:id="rId16"/>
     <sheet name="Underweight" sheetId="23" r:id="rId17"/>
     <sheet name="Child mortality" sheetId="24" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="16" state="hidden" r:id="rId19"/>
+    <sheet name="Rakesh_no_ingest" sheetId="16" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1154,6 +1154,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1208,16 +1217,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1532,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1572,7 +1572,7 @@
       <c r="H1" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="54" t="s">
         <v>161</v>
       </c>
     </row>
@@ -1590,16 +1590,16 @@
       <c r="D2" s="49" t="b">
         <v>0</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="71" t="s">
+      <c r="G2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="71" t="b">
+      <c r="H2" s="53" t="b">
         <v>0</v>
       </c>
-      <c r="I2" s="74" t="b">
+      <c r="I2" s="56" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1617,16 +1617,16 @@
       <c r="D3" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="75" t="s">
+      <c r="F3" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="53" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="76" t="b">
+      <c r="I3" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1644,7 +1644,7 @@
       <c r="D4" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="57" t="s">
         <v>156</v>
       </c>
       <c r="G4" s="44" t="s">
@@ -1653,7 +1653,7 @@
       <c r="H4" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I4" s="76" t="b">
+      <c r="I4" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
       <c r="D5" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="59" t="s">
         <v>157</v>
       </c>
       <c r="G5" s="44" t="s">
@@ -1679,7 +1679,7 @@
       <c r="H5" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I5" s="76" t="b">
+      <c r="I5" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1697,7 +1697,7 @@
       <c r="D6" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F6" s="78" t="s">
+      <c r="F6" s="57" t="s">
         <v>157</v>
       </c>
       <c r="G6" s="44" t="s">
@@ -1706,7 +1706,7 @@
       <c r="H6" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="76" t="b">
+      <c r="I6" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1724,7 +1724,7 @@
       <c r="D7" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="78" t="s">
+      <c r="F7" s="57" t="s">
         <v>157</v>
       </c>
       <c r="G7" s="44" t="s">
@@ -1733,7 +1733,7 @@
       <c r="H7" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I7" s="76" t="b">
+      <c r="I7" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1751,7 +1751,7 @@
       <c r="D8" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="78" t="s">
+      <c r="F8" s="57" t="s">
         <v>157</v>
       </c>
       <c r="G8" s="44" t="s">
@@ -1760,7 +1760,7 @@
       <c r="H8" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I8" s="76" t="b">
+      <c r="I8" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
       <c r="D9" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="78" t="s">
+      <c r="F9" s="57" t="s">
         <v>157</v>
       </c>
       <c r="G9" s="44" t="s">
@@ -1787,7 +1787,7 @@
       <c r="H9" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I9" s="76" t="b">
+      <c r="I9" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1805,7 +1805,7 @@
       <c r="D10" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F10" s="77" t="s">
+      <c r="F10" s="59" t="s">
         <v>158</v>
       </c>
       <c r="G10" s="44" t="s">
@@ -1814,7 +1814,7 @@
       <c r="H10" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I10" s="76" t="b">
+      <c r="I10" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1832,7 +1832,7 @@
       <c r="D11" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F11" s="78" t="s">
+      <c r="F11" s="57" t="s">
         <v>158</v>
       </c>
       <c r="G11" s="44" t="s">
@@ -1841,7 +1841,7 @@
       <c r="H11" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I11" s="76" t="b">
+      <c r="I11" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1859,7 +1859,7 @@
       <c r="D12" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="57" t="s">
         <v>158</v>
       </c>
       <c r="G12" s="44" t="s">
@@ -1868,7 +1868,7 @@
       <c r="H12" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I12" s="76" t="b">
+      <c r="I12" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       <c r="D13" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="57" t="s">
         <v>158</v>
       </c>
       <c r="G13" s="44" t="s">
@@ -1895,7 +1895,7 @@
       <c r="H13" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I13" s="76" t="b">
+      <c r="I13" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       <c r="D14" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="77" t="s">
+      <c r="F14" s="59" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="44" t="s">
@@ -1922,7 +1922,7 @@
       <c r="H14" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="76" t="b">
+      <c r="I14" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1940,7 +1940,7 @@
       <c r="D15" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="78" t="s">
+      <c r="F15" s="57" t="s">
         <v>5</v>
       </c>
       <c r="G15" s="44" t="s">
@@ -1949,7 +1949,7 @@
       <c r="H15" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I15" s="76" t="b">
+      <c r="I15" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1967,7 +1967,7 @@
       <c r="D16" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="78" t="s">
+      <c r="F16" s="57" t="s">
         <v>5</v>
       </c>
       <c r="G16" s="44" t="s">
@@ -1976,7 +1976,7 @@
       <c r="H16" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="76" t="b">
+      <c r="I16" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1994,7 +1994,7 @@
       <c r="D17" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="78" t="s">
+      <c r="F17" s="57" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="44" t="s">
@@ -2003,7 +2003,7 @@
       <c r="H17" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I17" s="76" t="b">
+      <c r="I17" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
       <c r="D18" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="77" t="s">
+      <c r="F18" s="59" t="s">
         <v>6</v>
       </c>
       <c r="G18" s="44" t="s">
@@ -2029,7 +2029,7 @@
       <c r="H18" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I18" s="76" t="b">
+      <c r="I18" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       <c r="D19" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="78" t="s">
+      <c r="F19" s="57" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="44" t="s">
@@ -2055,7 +2055,7 @@
       <c r="H19" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I19" s="76" t="b">
+      <c r="I19" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2072,7 +2072,7 @@
       <c r="D20" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="78" t="s">
+      <c r="F20" s="57" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="44" t="s">
@@ -2081,7 +2081,7 @@
       <c r="H20" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I20" s="76" t="b">
+      <c r="I20" s="58" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2098,7 +2098,7 @@
       <c r="D21" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="77" t="s">
+      <c r="F21" s="59" t="s">
         <v>159</v>
       </c>
       <c r="G21" s="44" t="s">
@@ -2107,7 +2107,7 @@
       <c r="H21" s="44" t="b">
         <v>0</v>
       </c>
-      <c r="I21" s="76" t="b">
+      <c r="I21" s="58" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2124,7 +2124,7 @@
       <c r="D22" s="48" t="b">
         <v>0</v>
       </c>
-      <c r="F22" s="79" t="s">
+      <c r="F22" s="60" t="s">
         <v>159</v>
       </c>
       <c r="G22" s="46" t="s">
@@ -2133,9 +2133,12 @@
       <c r="H22" s="46" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="80" t="b">
+      <c r="I22" s="61" t="b">
         <v>0</v>
       </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B23" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2160,65 +2163,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
     </row>
     <row r="2" spans="1:26" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:26" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -4726,34 +4729,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="54"/>
-      <c r="P43" s="54"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="53" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
       <c r="V43" s="6"/>
       <c r="W43" s="6"/>
       <c r="X43" s="6"/>
@@ -7257,57 +7260,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -9813,34 +9816,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="54"/>
-      <c r="P43" s="54"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="53" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AL43" s="2"/>
@@ -12285,17 +12288,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12317,59 +12320,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -14857,34 +14860,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="54"/>
-      <c r="P43" s="54"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="53" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -17314,17 +17317,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -17348,64 +17351,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="61"/>
-      <c r="B3" s="54"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -19863,34 +19866,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -22362,11 +22365,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -22375,6 +22373,11 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22397,44 +22400,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="61"/>
-      <c r="B3" s="54"/>
+      <c r="A3" s="70"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -24874,44 +24877,44 @@
       </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A45" s="63" t="s">
+      <c r="A45" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B45" s="63" t="s">
+      <c r="B45" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="63"/>
-      <c r="E45" s="63" t="s">
+      <c r="D45" s="72"/>
+      <c r="E45" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63" t="s">
+      <c r="F45" s="72"/>
+      <c r="G45" s="72"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63" t="s">
+      <c r="K45" s="72"/>
+      <c r="L45" s="72"/>
+      <c r="M45" s="72"/>
+      <c r="N45" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O45" s="63"/>
-      <c r="P45" s="63"/>
-      <c r="Q45" s="63"/>
-      <c r="R45" s="62" t="s">
+      <c r="O45" s="72"/>
+      <c r="P45" s="72"/>
+      <c r="Q45" s="72"/>
+      <c r="R45" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S45" s="62"/>
-      <c r="T45" s="62"/>
+      <c r="S45" s="71"/>
+      <c r="T45" s="71"/>
     </row>
     <row r="46" spans="1:26" ht="28" x14ac:dyDescent="0.35">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="72"/>
       <c r="C46" s="11" t="s">
         <v>7</v>
       </c>
@@ -27367,44 +27370,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63" t="s">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="62" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -29848,44 +29851,44 @@
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="63" t="s">
+      <c r="A42" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="63" t="s">
+      <c r="B42" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="63" t="s">
+      <c r="C42" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63" t="s">
+      <c r="D42" s="72"/>
+      <c r="E42" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="63" t="s">
+      <c r="F42" s="72"/>
+      <c r="G42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63" t="s">
+      <c r="K42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="M42" s="72"/>
+      <c r="N42" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="63"/>
-      <c r="P42" s="63"/>
-      <c r="Q42" s="63"/>
-      <c r="R42" s="62" t="s">
+      <c r="O42" s="72"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="72"/>
+      <c r="R42" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="62"/>
-      <c r="T42" s="62"/>
+      <c r="S42" s="71"/>
+      <c r="T42" s="71"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A43" s="63"/>
-      <c r="B43" s="63"/>
+      <c r="A43" s="72"/>
+      <c r="B43" s="72"/>
       <c r="C43" s="11" t="s">
         <v>7</v>
       </c>
@@ -32342,6 +32345,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -32349,13 +32359,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -32373,44 +32376,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63" t="s">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="62" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -34854,44 +34857,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63" t="s">
+      <c r="D43" s="72"/>
+      <c r="E43" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63" t="s">
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63" t="s">
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="62" t="s">
+      <c r="O43" s="72"/>
+      <c r="P43" s="72"/>
+      <c r="Q43" s="72"/>
+      <c r="R43" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="62"/>
-      <c r="T43" s="62"/>
+      <c r="S43" s="71"/>
+      <c r="T43" s="71"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="63"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="72"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -37348,6 +37351,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -37355,13 +37365,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -37378,44 +37381,44 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="1:21" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="63" t="s">
+      <c r="C2" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63" t="s">
+      <c r="D2" s="72"/>
+      <c r="E2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63" t="s">
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63" t="s">
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="62" t="s">
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
+      <c r="S2" s="71"/>
+      <c r="T2" s="71"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
       <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
@@ -39859,44 +39862,44 @@
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A43" s="63" t="s">
+      <c r="A43" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="63" t="s">
+      <c r="B43" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="63"/>
-      <c r="E43" s="63" t="s">
+      <c r="D43" s="72"/>
+      <c r="E43" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63" t="s">
+      <c r="F43" s="72"/>
+      <c r="G43" s="72"/>
+      <c r="H43" s="72"/>
+      <c r="I43" s="72"/>
+      <c r="J43" s="72" t="s">
         <v>117</v>
       </c>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63" t="s">
+      <c r="K43" s="72"/>
+      <c r="L43" s="72"/>
+      <c r="M43" s="72"/>
+      <c r="N43" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="63"/>
-      <c r="P43" s="63"/>
-      <c r="Q43" s="63"/>
-      <c r="R43" s="62" t="s">
+      <c r="O43" s="72"/>
+      <c r="P43" s="72"/>
+      <c r="Q43" s="72"/>
+      <c r="R43" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="62"/>
-      <c r="T43" s="62"/>
+      <c r="S43" s="71"/>
+      <c r="T43" s="71"/>
     </row>
     <row r="44" spans="1:21" ht="42" x14ac:dyDescent="0.35">
-      <c r="A44" s="63"/>
-      <c r="B44" s="63"/>
+      <c r="A44" s="72"/>
+      <c r="B44" s="72"/>
       <c r="C44" s="11" t="s">
         <v>7</v>
       </c>
@@ -42353,6 +42356,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R43:T43"/>
     <mergeCell ref="A43:A44"/>
     <mergeCell ref="B43:B44"/>
@@ -42360,13 +42370,6 @@
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="J43:M43"/>
     <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42376,8 +42379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AJ35" sqref="AJ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42394,157 +42397,157 @@
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
-      <c r="G2" s="64" t="s">
+      <c r="G2" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="65" t="s">
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="66"/>
-      <c r="X2" s="66"/>
-      <c r="Y2" s="66"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="64" t="s">
+      <c r="R2" s="75"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AB2" s="64"/>
-      <c r="AC2" s="64"/>
-      <c r="AD2" s="64"/>
-      <c r="AE2" s="64"/>
-      <c r="AF2" s="64"/>
-      <c r="AG2" s="64"/>
-      <c r="AH2" s="64"/>
-      <c r="AI2" s="64"/>
-      <c r="AJ2" s="64"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="73"/>
       <c r="AK2" s="29"/>
       <c r="AL2" s="29"/>
       <c r="AM2" s="29"/>
       <c r="AN2" s="29"/>
-      <c r="AO2" s="68" t="s">
+      <c r="AO2" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="AP2" s="69"/>
-      <c r="AQ2" s="69"/>
-      <c r="AR2" s="69"/>
-      <c r="AS2" s="69"/>
-      <c r="AT2" s="70"/>
+      <c r="AP2" s="78"/>
+      <c r="AQ2" s="78"/>
+      <c r="AR2" s="78"/>
+      <c r="AS2" s="78"/>
+      <c r="AT2" s="79"/>
       <c r="AU2" s="23"/>
       <c r="AV2" s="23"/>
       <c r="AW2" s="23"/>
       <c r="AX2" s="23"/>
-      <c r="AY2" s="64" t="s">
+      <c r="AY2" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AZ2" s="64"/>
-      <c r="BA2" s="64"/>
-      <c r="BB2" s="64"/>
-      <c r="BC2" s="64"/>
-      <c r="BD2" s="64"/>
-      <c r="BE2" s="64"/>
-      <c r="BF2" s="64"/>
-      <c r="BG2" s="64"/>
-      <c r="BH2" s="64"/>
-      <c r="BI2" s="64"/>
+      <c r="AZ2" s="73"/>
+      <c r="BA2" s="73"/>
+      <c r="BB2" s="73"/>
+      <c r="BC2" s="73"/>
+      <c r="BD2" s="73"/>
+      <c r="BE2" s="73"/>
+      <c r="BF2" s="73"/>
+      <c r="BG2" s="73"/>
+      <c r="BH2" s="73"/>
+      <c r="BI2" s="73"/>
     </row>
     <row r="3" spans="1:62" x14ac:dyDescent="0.35">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64" t="s">
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64" t="s">
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64" t="s">
+      <c r="M3" s="73"/>
+      <c r="N3" s="73"/>
+      <c r="O3" s="73"/>
+      <c r="P3" s="73"/>
+      <c r="Q3" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="R3" s="64"/>
-      <c r="S3" s="64"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64" t="s">
+      <c r="R3" s="73"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="73"/>
+      <c r="V3" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="64"/>
-      <c r="AA3" s="64" t="s">
+      <c r="W3" s="73"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="73"/>
+      <c r="Z3" s="73"/>
+      <c r="AA3" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="AB3" s="64"/>
-      <c r="AC3" s="64"/>
-      <c r="AD3" s="64"/>
-      <c r="AE3" s="64"/>
-      <c r="AF3" s="64" t="s">
+      <c r="AB3" s="73"/>
+      <c r="AC3" s="73"/>
+      <c r="AD3" s="73"/>
+      <c r="AE3" s="73"/>
+      <c r="AF3" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="AG3" s="64"/>
-      <c r="AH3" s="64"/>
-      <c r="AI3" s="64"/>
-      <c r="AJ3" s="64"/>
-      <c r="AK3" s="64" t="s">
+      <c r="AG3" s="73"/>
+      <c r="AH3" s="73"/>
+      <c r="AI3" s="73"/>
+      <c r="AJ3" s="73"/>
+      <c r="AK3" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="AL3" s="64"/>
-      <c r="AM3" s="64"/>
-      <c r="AN3" s="64"/>
-      <c r="AO3" s="64"/>
-      <c r="AP3" s="64" t="s">
+      <c r="AL3" s="73"/>
+      <c r="AM3" s="73"/>
+      <c r="AN3" s="73"/>
+      <c r="AO3" s="73"/>
+      <c r="AP3" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="AQ3" s="64"/>
-      <c r="AR3" s="64"/>
-      <c r="AS3" s="64"/>
-      <c r="AT3" s="64"/>
-      <c r="AU3" s="64" t="s">
+      <c r="AQ3" s="73"/>
+      <c r="AR3" s="73"/>
+      <c r="AS3" s="73"/>
+      <c r="AT3" s="73"/>
+      <c r="AU3" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AV3" s="64"/>
-      <c r="AW3" s="64"/>
-      <c r="AX3" s="64"/>
-      <c r="AY3" s="64"/>
-      <c r="AZ3" s="64" t="s">
+      <c r="AV3" s="73"/>
+      <c r="AW3" s="73"/>
+      <c r="AX3" s="73"/>
+      <c r="AY3" s="73"/>
+      <c r="AZ3" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="BA3" s="64"/>
-      <c r="BB3" s="64"/>
-      <c r="BC3" s="64"/>
-      <c r="BD3" s="64"/>
-      <c r="BE3" s="64" t="s">
+      <c r="BA3" s="73"/>
+      <c r="BB3" s="73"/>
+      <c r="BC3" s="73"/>
+      <c r="BD3" s="73"/>
+      <c r="BE3" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="BF3" s="64"/>
-      <c r="BG3" s="64"/>
-      <c r="BH3" s="64"/>
-      <c r="BI3" s="64"/>
+      <c r="BF3" s="73"/>
+      <c r="BG3" s="73"/>
+      <c r="BH3" s="73"/>
+      <c r="BI3" s="73"/>
       <c r="BJ3" s="1"/>
     </row>
     <row r="4" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -47902,19 +47905,24 @@
         <v>39.265300000000003</v>
       </c>
       <c r="AF34" s="28">
-        <v>35122.5</v>
+        <f>35122.5/1000</f>
+        <v>35.122500000000002</v>
       </c>
       <c r="AG34" s="28">
-        <v>4664.2</v>
+        <f>4664.2/1000</f>
+        <v>4.6642000000000001</v>
       </c>
       <c r="AH34" s="28">
-        <v>39623</v>
+        <f>39623/1000</f>
+        <v>39.622999999999998</v>
       </c>
       <c r="AI34" s="28">
-        <v>15812.300000000001</v>
+        <f>15812.3/1000</f>
+        <v>15.812299999999999</v>
       </c>
       <c r="AJ34" s="28">
-        <v>9358.5999999999985</v>
+        <f>9358.6/1000</f>
+        <v>9.3586000000000009</v>
       </c>
       <c r="AK34" s="28">
         <v>30.456799999999998</v>
@@ -48065,160 +48073,160 @@
       <c r="D36" s="23"/>
       <c r="E36" s="23"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="64" t="s">
+      <c r="G36" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-      <c r="K36" s="64"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
-      <c r="P36" s="64"/>
-      <c r="Q36" s="65" t="s">
+      <c r="H36" s="73"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="73"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="R36" s="66"/>
-      <c r="S36" s="66"/>
-      <c r="T36" s="66"/>
-      <c r="U36" s="66"/>
-      <c r="V36" s="66"/>
-      <c r="W36" s="66"/>
-      <c r="X36" s="66"/>
-      <c r="Y36" s="66"/>
-      <c r="Z36" s="67"/>
-      <c r="AA36" s="64" t="s">
+      <c r="R36" s="75"/>
+      <c r="S36" s="75"/>
+      <c r="T36" s="75"/>
+      <c r="U36" s="75"/>
+      <c r="V36" s="75"/>
+      <c r="W36" s="75"/>
+      <c r="X36" s="75"/>
+      <c r="Y36" s="75"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="AB36" s="64"/>
-      <c r="AC36" s="64"/>
-      <c r="AD36" s="64"/>
-      <c r="AE36" s="64"/>
-      <c r="AF36" s="64"/>
-      <c r="AG36" s="64"/>
-      <c r="AH36" s="64"/>
-      <c r="AI36" s="64"/>
-      <c r="AJ36" s="64"/>
+      <c r="AB36" s="73"/>
+      <c r="AC36" s="73"/>
+      <c r="AD36" s="73"/>
+      <c r="AE36" s="73"/>
+      <c r="AF36" s="73"/>
+      <c r="AG36" s="73"/>
+      <c r="AH36" s="73"/>
+      <c r="AI36" s="73"/>
+      <c r="AJ36" s="73"/>
       <c r="AK36" s="29"/>
       <c r="AL36" s="29"/>
       <c r="AM36" s="29"/>
       <c r="AN36" s="29"/>
-      <c r="AO36" s="68" t="s">
+      <c r="AO36" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="AP36" s="69"/>
-      <c r="AQ36" s="69"/>
-      <c r="AR36" s="69"/>
-      <c r="AS36" s="69"/>
-      <c r="AT36" s="70"/>
+      <c r="AP36" s="78"/>
+      <c r="AQ36" s="78"/>
+      <c r="AR36" s="78"/>
+      <c r="AS36" s="78"/>
+      <c r="AT36" s="79"/>
       <c r="AU36" s="23"/>
       <c r="AV36" s="23"/>
       <c r="AW36" s="23"/>
       <c r="AX36" s="23"/>
-      <c r="AY36" s="64" t="s">
+      <c r="AY36" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AZ36" s="64"/>
-      <c r="BA36" s="64"/>
-      <c r="BB36" s="64"/>
-      <c r="BC36" s="64"/>
-      <c r="BD36" s="64"/>
-      <c r="BE36" s="64"/>
-      <c r="BF36" s="64"/>
-      <c r="BG36" s="64"/>
-      <c r="BH36" s="64"/>
-      <c r="BI36" s="64"/>
+      <c r="AZ36" s="73"/>
+      <c r="BA36" s="73"/>
+      <c r="BB36" s="73"/>
+      <c r="BC36" s="73"/>
+      <c r="BD36" s="73"/>
+      <c r="BE36" s="73"/>
+      <c r="BF36" s="73"/>
+      <c r="BG36" s="73"/>
+      <c r="BH36" s="73"/>
+      <c r="BI36" s="73"/>
     </row>
     <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B37" s="64" t="s">
+      <c r="B37" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64" t="s">
+      <c r="C37" s="73"/>
+      <c r="D37" s="73"/>
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-      <c r="K37" s="64"/>
-      <c r="L37" s="64" t="s">
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="M37" s="64"/>
-      <c r="N37" s="64"/>
-      <c r="O37" s="64"/>
-      <c r="P37" s="64"/>
-      <c r="Q37" s="64" t="s">
+      <c r="M37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="R37" s="64"/>
-      <c r="S37" s="64"/>
-      <c r="T37" s="64"/>
-      <c r="U37" s="64"/>
-      <c r="V37" s="64" t="s">
+      <c r="R37" s="73"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="W37" s="64"/>
-      <c r="X37" s="64"/>
-      <c r="Y37" s="64"/>
-      <c r="Z37" s="64"/>
-      <c r="AA37" s="64" t="s">
+      <c r="W37" s="73"/>
+      <c r="X37" s="73"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="73"/>
+      <c r="AA37" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="AB37" s="64"/>
-      <c r="AC37" s="64"/>
-      <c r="AD37" s="64"/>
-      <c r="AE37" s="64"/>
-      <c r="AF37" s="64" t="s">
+      <c r="AB37" s="73"/>
+      <c r="AC37" s="73"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="73"/>
+      <c r="AF37" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="AG37" s="64"/>
-      <c r="AH37" s="64"/>
-      <c r="AI37" s="64"/>
-      <c r="AJ37" s="64"/>
-      <c r="AK37" s="64" t="s">
+      <c r="AG37" s="73"/>
+      <c r="AH37" s="73"/>
+      <c r="AI37" s="73"/>
+      <c r="AJ37" s="73"/>
+      <c r="AK37" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="AL37" s="64"/>
-      <c r="AM37" s="64"/>
-      <c r="AN37" s="64"/>
-      <c r="AO37" s="64"/>
-      <c r="AP37" s="64" t="s">
+      <c r="AL37" s="73"/>
+      <c r="AM37" s="73"/>
+      <c r="AN37" s="73"/>
+      <c r="AO37" s="73"/>
+      <c r="AP37" s="73" t="s">
         <v>23</v>
       </c>
-      <c r="AQ37" s="64"/>
-      <c r="AR37" s="64"/>
-      <c r="AS37" s="64"/>
-      <c r="AT37" s="64"/>
-      <c r="AU37" s="64" t="s">
+      <c r="AQ37" s="73"/>
+      <c r="AR37" s="73"/>
+      <c r="AS37" s="73"/>
+      <c r="AT37" s="73"/>
+      <c r="AU37" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="AV37" s="64"/>
-      <c r="AW37" s="64"/>
-      <c r="AX37" s="64"/>
-      <c r="AY37" s="64"/>
-      <c r="AZ37" s="64" t="s">
+      <c r="AV37" s="73"/>
+      <c r="AW37" s="73"/>
+      <c r="AX37" s="73"/>
+      <c r="AY37" s="73"/>
+      <c r="AZ37" s="73" t="s">
         <v>11</v>
       </c>
-      <c r="BA37" s="64"/>
-      <c r="BB37" s="64"/>
-      <c r="BC37" s="64"/>
-      <c r="BD37" s="64"/>
-      <c r="BE37" s="64" t="s">
+      <c r="BA37" s="73"/>
+      <c r="BB37" s="73"/>
+      <c r="BC37" s="73"/>
+      <c r="BD37" s="73"/>
+      <c r="BE37" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="BF37" s="64"/>
-      <c r="BG37" s="64"/>
-      <c r="BH37" s="64"/>
-      <c r="BI37" s="64"/>
+      <c r="BF37" s="73"/>
+      <c r="BG37" s="73"/>
+      <c r="BH37" s="73"/>
+      <c r="BI37" s="73"/>
       <c r="BJ37" s="1"/>
     </row>
     <row r="38" spans="1:62" ht="42" x14ac:dyDescent="0.35">
@@ -53784,6 +53792,28 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE3:BI3"/>
+    <mergeCell ref="G36:P36"/>
+    <mergeCell ref="Q36:Z36"/>
+    <mergeCell ref="AA36:AJ36"/>
+    <mergeCell ref="AO36:AT36"/>
+    <mergeCell ref="AY36:BI36"/>
+    <mergeCell ref="AA3:AE3"/>
+    <mergeCell ref="AF3:AJ3"/>
+    <mergeCell ref="AK3:AO3"/>
+    <mergeCell ref="AP3:AT3"/>
+    <mergeCell ref="AU3:AY3"/>
+    <mergeCell ref="AZ3:BD3"/>
     <mergeCell ref="BE37:BI37"/>
     <mergeCell ref="B37:F37"/>
     <mergeCell ref="G37:K37"/>
@@ -53796,28 +53826,6 @@
     <mergeCell ref="AP37:AT37"/>
     <mergeCell ref="AU37:AY37"/>
     <mergeCell ref="AZ37:BD37"/>
-    <mergeCell ref="BE3:BI3"/>
-    <mergeCell ref="G36:P36"/>
-    <mergeCell ref="Q36:Z36"/>
-    <mergeCell ref="AA36:AJ36"/>
-    <mergeCell ref="AO36:AT36"/>
-    <mergeCell ref="AY36:BI36"/>
-    <mergeCell ref="AA3:AE3"/>
-    <mergeCell ref="AF3:AJ3"/>
-    <mergeCell ref="AK3:AO3"/>
-    <mergeCell ref="AP3:AT3"/>
-    <mergeCell ref="AU3:AY3"/>
-    <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -53837,44 +53845,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63" t="s">
+      <c r="D1" s="72"/>
+      <c r="E1" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="63" t="s">
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63" t="s">
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="63"/>
-      <c r="P1" s="63"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
       <c r="Q1" s="10"/>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
+      <c r="S1" s="71"/>
+      <c r="T1" s="71"/>
     </row>
     <row r="2" spans="1:20" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="63"/>
-      <c r="B2" s="63"/>
+      <c r="A2" s="72"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="11" t="s">
         <v>7</v>
       </c>
@@ -56234,7 +56242,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A42" sqref="A42:U43"/>
+      <selection pane="topRight" activeCell="C3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -56246,64 +56254,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -58755,34 +58763,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -61183,6 +61191,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -61191,11 +61204,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -61207,7 +61215,7 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="C3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -61219,44 +61227,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
+      <c r="A3" s="63"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
@@ -63729,44 +63737,44 @@
       <c r="T41" s="6"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A42" s="54" t="s">
+      <c r="A42" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B42" s="54" t="s">
+      <c r="B42" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
-      <c r="A43" s="54"/>
-      <c r="B43" s="54"/>
+      <c r="A43" s="63"/>
+      <c r="B43" s="63"/>
       <c r="C43" s="1" t="s">
         <v>7</v>
       </c>
@@ -66158,6 +66166,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
@@ -66165,13 +66180,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -66184,7 +66192,7 @@
   <sheetViews>
     <sheetView zoomScale="62" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z11" sqref="Z11"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -66194,57 +66202,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
+      <c r="A1" s="65"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -68708,34 +68716,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -71133,17 +71141,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -71154,7 +71162,7 @@
   <dimension ref="A1:U80"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L76" sqref="L76"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -71164,59 +71172,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-      <c r="Q1" s="59"/>
-      <c r="R1" s="59"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -73724,34 +73732,34 @@
       <c r="A43" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54" t="s">
+      <c r="D43" s="63"/>
+      <c r="E43" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54" t="s">
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="63"/>
+      <c r="N43" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O43" s="54"/>
-      <c r="P43" s="54"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="53" t="s">
+      <c r="O43" s="63"/>
+      <c r="P43" s="63"/>
+      <c r="Q43" s="63"/>
+      <c r="R43" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S43" s="53"/>
-      <c r="T43" s="53"/>
+      <c r="S43" s="62"/>
+      <c r="T43" s="62"/>
     </row>
     <row r="44" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A44" s="18"/>
@@ -76146,17 +76154,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -76180,57 +76188,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="41.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -78738,34 +78746,34 @@
       <c r="A44" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54" t="s">
+      <c r="D44" s="63"/>
+      <c r="E44" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54" t="s">
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="54" t="s">
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="63"/>
+      <c r="N44" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O44" s="54"/>
-      <c r="P44" s="54"/>
-      <c r="Q44" s="54"/>
-      <c r="R44" s="53" t="s">
+      <c r="O44" s="63"/>
+      <c r="P44" s="63"/>
+      <c r="Q44" s="63"/>
+      <c r="R44" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S44" s="53"/>
-      <c r="T44" s="53"/>
+      <c r="S44" s="62"/>
+      <c r="T44" s="62"/>
     </row>
     <row r="45" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A45" s="18"/>
@@ -81414,17 +81422,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -81447,57 +81455,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
     </row>
     <row r="2" spans="1:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -83959,34 +83967,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -86446,17 +86454,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -86477,24 +86485,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
+      <c r="A1" s="69"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
@@ -86503,34 +86511,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -88976,34 +88984,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -91421,17 +91429,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -91455,34 +91463,34 @@
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54" t="s">
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54" t="s">
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="53" t="s">
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A3" s="18"/>
@@ -93942,34 +93950,34 @@
       <c r="A42" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="54" t="s">
+      <c r="C42" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="63"/>
+      <c r="E42" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54" t="s">
+      <c r="K42" s="63"/>
+      <c r="L42" s="63"/>
+      <c r="M42" s="63"/>
+      <c r="N42" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="O42" s="54"/>
-      <c r="P42" s="54"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="53" t="s">
+      <c r="O42" s="63"/>
+      <c r="P42" s="63"/>
+      <c r="Q42" s="63"/>
+      <c r="R42" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="S42" s="53"/>
-      <c r="T42" s="53"/>
+      <c r="S42" s="62"/>
+      <c r="T42" s="62"/>
     </row>
     <row r="43" spans="1:21" ht="42" x14ac:dyDescent="0.35">
       <c r="A43" s="18"/>
@@ -96426,16 +96434,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified values child mortality all india nfhs 4
</commit_message>
<xml_diff>
--- a/datasets/Equity_Analysis.xlsx
+++ b/datasets/Equity_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16f1c7c3db740efb/UNICEF/india_co/nfhs_2022/ico-nfhs-multipage/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9794DDE4-6943-4539-9269-61CDC836FDC6}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="13_ncr:1_{4F8A55A9-1CCB-4AC9-9D7C-98FE59C7C53F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3929F08-83BE-4925-B40D-EE611963A5BC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="881" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="881" firstSheet="8" activeTab="17" xr2:uid="{F81DF295-D280-4E86-B212-908814D88627}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Wasted" sheetId="22" r:id="rId16"/>
     <sheet name="Underweight" sheetId="23" r:id="rId17"/>
     <sheet name="Child mortality" sheetId="24" r:id="rId18"/>
-    <sheet name="Rakesh_no_ingest" sheetId="16" r:id="rId19"/>
+    <sheet name="Rakesh_no_ingest" sheetId="16" state="hidden" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1044,7 +1044,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1217,7 +1217,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1532,9 +1531,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5A8E82-BFD9-49B2-A6E2-468C6F875F62}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2136,9 +2135,6 @@
       <c r="I22" s="61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B23" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12288,17 +12284,17 @@
     <sortCondition ref="AC1:AC92"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17317,17 +17313,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:T2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -22365,6 +22361,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
@@ -22373,11 +22374,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32345,6 +32341,13 @@
     <sortCondition ref="A44:A79"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -32352,13 +32355,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -37351,6 +37347,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -37358,13 +37361,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42356,6 +42352,13 @@
     <sortCondition ref="A45:A80"/>
   </sortState>
   <mergeCells count="14">
+    <mergeCell ref="R43:T43"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -42363,13 +42366,6 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R43:T43"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -42379,8 +42375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3260E9C-5C50-46D3-8D52-12A1BD072B1C}">
   <dimension ref="A2:BJ69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AJ35" sqref="AJ35"/>
+    <sheetView tabSelected="1" topLeftCell="Q2" workbookViewId="0">
+      <selection activeCell="AF34" sqref="AF34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47905,24 +47901,19 @@
         <v>39.265300000000003</v>
       </c>
       <c r="AF34" s="28">
-        <f>35122.5/1000</f>
-        <v>35.122500000000002</v>
+        <v>31.3</v>
       </c>
       <c r="AG34" s="28">
-        <f>4664.2/1000</f>
-        <v>4.6642000000000001</v>
+        <v>13.1</v>
       </c>
       <c r="AH34" s="28">
-        <f>39623/1000</f>
-        <v>39.622999999999998</v>
+        <v>44.4</v>
       </c>
       <c r="AI34" s="28">
-        <f>15812.3/1000</f>
-        <v>15.812299999999999</v>
+        <v>13.4</v>
       </c>
       <c r="AJ34" s="28">
-        <f>9358.6/1000</f>
-        <v>9.3586000000000009</v>
+        <v>57.2</v>
       </c>
       <c r="AK34" s="28">
         <v>30.456799999999998</v>
@@ -53792,16 +53783,18 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="Q3:U3"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="G2:P2"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="AA2:AJ2"/>
-    <mergeCell ref="AO2:AT2"/>
-    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="BE37:BI37"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="G37:K37"/>
+    <mergeCell ref="L37:P37"/>
+    <mergeCell ref="Q37:U37"/>
+    <mergeCell ref="V37:Z37"/>
+    <mergeCell ref="AA37:AE37"/>
+    <mergeCell ref="AF37:AJ37"/>
+    <mergeCell ref="AK37:AO37"/>
+    <mergeCell ref="AP37:AT37"/>
+    <mergeCell ref="AU37:AY37"/>
+    <mergeCell ref="AZ37:BD37"/>
     <mergeCell ref="BE3:BI3"/>
     <mergeCell ref="G36:P36"/>
     <mergeCell ref="Q36:Z36"/>
@@ -53814,18 +53807,16 @@
     <mergeCell ref="AP3:AT3"/>
     <mergeCell ref="AU3:AY3"/>
     <mergeCell ref="AZ3:BD3"/>
-    <mergeCell ref="BE37:BI37"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="G37:K37"/>
-    <mergeCell ref="L37:P37"/>
-    <mergeCell ref="Q37:U37"/>
-    <mergeCell ref="V37:Z37"/>
-    <mergeCell ref="AA37:AE37"/>
-    <mergeCell ref="AF37:AJ37"/>
-    <mergeCell ref="AK37:AO37"/>
-    <mergeCell ref="AP37:AT37"/>
-    <mergeCell ref="AU37:AY37"/>
-    <mergeCell ref="AZ37:BD37"/>
+    <mergeCell ref="G2:P2"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="AA2:AJ2"/>
+    <mergeCell ref="AO2:AT2"/>
+    <mergeCell ref="AY2:BI2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="Q3:U3"/>
+    <mergeCell ref="V3:Z3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -61191,11 +61182,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A1:R1"/>
@@ -61204,6 +61190,11 @@
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -66166,6 +66157,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="R2:T2"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R42:T42"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="B42:B43"/>
@@ -66173,13 +66171,6 @@
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="J42:M42"/>
     <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R2:T2"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:Q2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -71141,17 +71132,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
+    <mergeCell ref="R42:T42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="R42:T42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -76154,17 +76145,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="N43:Q43"/>
+    <mergeCell ref="R43:T43"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="N43:Q43"/>
-    <mergeCell ref="R43:T43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -81422,17 +81413,17 @@
     <sortCondition ref="C89:C119"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="J44:M44"/>
-    <mergeCell ref="R44:T44"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="J44:M44"/>
+    <mergeCell ref="R44:T44"/>
+    <mergeCell ref="N44:Q44"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -86454,17 +86445,17 @@
     <sortCondition ref="A43:A79"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -91429,17 +91420,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -96434,16 +96425,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="R42:T42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="N42:Q42"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:I2"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="R42:T42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="N42:Q42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>